<commit_message>
icmecat added psp event
</commit_message>
<xml_diff>
--- a/icmecat/HELCATS_ICMECAT_v20.xlsx
+++ b/icmecat/HELCATS_ICMECAT_v20.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S705"/>
+  <dimension ref="A1:S706"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -50442,6 +50442,77 @@
         <v>-3.61</v>
       </c>
     </row>
+    <row r="706">
+      <c r="A706" s="1" t="n">
+        <v>704</v>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>ICME_PSP_MOESTL_20181111_01</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>PSP</t>
+        </is>
+      </c>
+      <c r="D706" t="inlineStr">
+        <is>
+          <t>2018-11-11T17:39Z</t>
+        </is>
+      </c>
+      <c r="E706" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2018-11-11T23:51Z </t>
+        </is>
+      </c>
+      <c r="F706" t="inlineStr">
+        <is>
+          <t>2018-11-12T05:59Z</t>
+        </is>
+      </c>
+      <c r="G706" t="inlineStr">
+        <is>
+          <t>9999-99-99T99:99Z</t>
+        </is>
+      </c>
+      <c r="H706" t="n">
+        <v>98.8</v>
+      </c>
+      <c r="I706" t="n">
+        <v>59.1</v>
+      </c>
+      <c r="J706" t="n">
+        <v>12.33</v>
+      </c>
+      <c r="K706" t="n">
+        <v>98.8</v>
+      </c>
+      <c r="L706" t="n">
+        <v>82.40000000000001</v>
+      </c>
+      <c r="M706" t="n">
+        <v>13</v>
+      </c>
+      <c r="N706" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="O706" t="n">
+        <v>-34</v>
+      </c>
+      <c r="P706" t="n">
+        <v>6.13</v>
+      </c>
+      <c r="Q706" t="n">
+        <v>0.2574</v>
+      </c>
+      <c r="R706" t="n">
+        <v>114.87</v>
+      </c>
+      <c r="S706" t="n">
+        <v>-1.05</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed Wind plasma spikes helcats
</commit_message>
<xml_diff>
--- a/icmecat/HELCATS_ICMECAT_v20.xlsx
+++ b/icmecat/HELCATS_ICMECAT_v20.xlsx
@@ -609,10 +609,10 @@
         <v>2.5</v>
       </c>
       <c r="N2" t="n">
-        <v>361.5</v>
+        <v>361.1</v>
       </c>
       <c r="O2" t="n">
-        <v>16.3</v>
+        <v>12.9</v>
       </c>
       <c r="P2" t="n">
         <v>20.02</v>
@@ -642,25 +642,25 @@
         <v>3.5</v>
       </c>
       <c r="Y2" t="n">
-        <v>362</v>
+        <v>361.7</v>
       </c>
       <c r="Z2" t="n">
-        <v>15.5</v>
+        <v>11.8</v>
       </c>
       <c r="AA2" t="n">
         <v>-35.6</v>
       </c>
       <c r="AB2" t="n">
-        <v>1.2</v>
+        <v>1.1</v>
       </c>
       <c r="AC2" t="n">
-        <v>2.7</v>
+        <v>0.5</v>
       </c>
       <c r="AD2" t="n">
-        <v>5.2</v>
+        <v>5</v>
       </c>
       <c r="AE2" t="n">
-        <v>4.2</v>
+        <v>2.1</v>
       </c>
       <c r="AF2" t="n">
         <v>15652.6</v>
@@ -1216,10 +1216,10 @@
         <v>5.4</v>
       </c>
       <c r="N7" t="n">
-        <v>455.3</v>
+        <v>454.4</v>
       </c>
       <c r="O7" t="n">
-        <v>28.8</v>
+        <v>25.6</v>
       </c>
       <c r="P7" t="n">
         <v>10.97</v>
@@ -1258,16 +1258,16 @@
         <v>-4.5</v>
       </c>
       <c r="AB7" t="n">
-        <v>4.5</v>
+        <v>4.4</v>
       </c>
       <c r="AC7" t="n">
-        <v>3.4</v>
+        <v>3.3</v>
       </c>
       <c r="AD7" t="n">
-        <v>12.5</v>
+        <v>12.4</v>
       </c>
       <c r="AE7" t="n">
-        <v>9.800000000000001</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="AF7" t="n">
         <v>25979.3</v>
@@ -1276,22 +1276,22 @@
         <v>13532.3</v>
       </c>
       <c r="AH7" t="n">
-        <v>437.2</v>
+        <v>434.3</v>
       </c>
       <c r="AI7" t="n">
-        <v>40</v>
+        <v>31.9</v>
       </c>
       <c r="AJ7" t="n">
-        <v>25.5</v>
+        <v>24.4</v>
       </c>
       <c r="AK7" t="n">
-        <v>12.2</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="AL7" t="n">
-        <v>8.699999999999999</v>
+        <v>8</v>
       </c>
       <c r="AM7" t="n">
-        <v>9.300000000000001</v>
+        <v>7.2</v>
       </c>
     </row>
     <row r="8">
@@ -1345,10 +1345,10 @@
         <v>1.1</v>
       </c>
       <c r="N8" t="n">
-        <v>350</v>
+        <v>349.7</v>
       </c>
       <c r="O8" t="n">
-        <v>13.4</v>
+        <v>11.1</v>
       </c>
       <c r="P8" t="n">
         <v>17.27</v>
@@ -1378,19 +1378,17 @@
         <v>1</v>
       </c>
       <c r="Y8" t="n">
-        <v>350</v>
+        <v>349.7</v>
       </c>
       <c r="Z8" t="n">
-        <v>13.4</v>
-      </c>
-      <c r="AA8" t="n">
-        <v>-4.6</v>
-      </c>
+        <v>11.1</v>
+      </c>
+      <c r="AA8" t="inlineStr"/>
       <c r="AB8" t="n">
         <v>1.2</v>
       </c>
       <c r="AC8" t="n">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="AD8" t="n">
         <v>5.9</v>
@@ -1504,16 +1502,16 @@
         <v>17.8</v>
       </c>
       <c r="AB9" t="n">
-        <v>1.3</v>
+        <v>1.1</v>
       </c>
       <c r="AC9" t="n">
-        <v>2.4</v>
+        <v>0.1</v>
       </c>
       <c r="AD9" t="n">
-        <v>3.1</v>
+        <v>2.7</v>
       </c>
       <c r="AE9" t="n">
-        <v>5.9</v>
+        <v>0.2</v>
       </c>
       <c r="AF9" t="n">
         <v>89951.89999999999</v>
@@ -1579,10 +1577,10 @@
         <v>1.2</v>
       </c>
       <c r="N10" t="n">
-        <v>466.4</v>
+        <v>467.5</v>
       </c>
       <c r="O10" t="n">
-        <v>24.9</v>
+        <v>16.7</v>
       </c>
       <c r="P10" t="n">
         <v>11.28</v>
@@ -1612,10 +1610,10 @@
         <v>5.2</v>
       </c>
       <c r="Y10" t="n">
-        <v>466.4</v>
+        <v>467.5</v>
       </c>
       <c r="Z10" t="n">
-        <v>24.9</v>
+        <v>16.7</v>
       </c>
       <c r="AA10" t="n">
         <v>-30.8</v>
@@ -1741,13 +1739,13 @@
         <v>0.9</v>
       </c>
       <c r="AC11" t="n">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="AD11" t="n">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="AE11" t="n">
-        <v>2.7</v>
+        <v>1.7</v>
       </c>
       <c r="AF11" t="n">
         <v>15013.6</v>
@@ -1825,10 +1823,10 @@
         <v>0.6</v>
       </c>
       <c r="N12" t="n">
-        <v>398.6</v>
+        <v>398.2</v>
       </c>
       <c r="O12" t="n">
-        <v>25.8</v>
+        <v>21.9</v>
       </c>
       <c r="P12" t="n">
         <v>18</v>
@@ -1858,25 +1856,25 @@
         <v>1.6</v>
       </c>
       <c r="Y12" t="n">
-        <v>390.4</v>
+        <v>389.9</v>
       </c>
       <c r="Z12" t="n">
-        <v>22.5</v>
+        <v>16.1</v>
       </c>
       <c r="AA12" t="n">
         <v>23.1</v>
       </c>
       <c r="AB12" t="n">
-        <v>1.3</v>
+        <v>1.1</v>
       </c>
       <c r="AC12" t="n">
-        <v>4.8</v>
+        <v>0.3</v>
       </c>
       <c r="AD12" t="n">
-        <v>4.5</v>
+        <v>4.2</v>
       </c>
       <c r="AE12" t="n">
-        <v>4.8</v>
+        <v>0.8</v>
       </c>
       <c r="AF12" t="n">
         <v>32202.8</v>
@@ -1954,10 +1952,10 @@
         <v>1.4</v>
       </c>
       <c r="N13" t="n">
-        <v>337.9</v>
+        <v>337.4</v>
       </c>
       <c r="O13" t="n">
-        <v>12.7</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="P13" t="n">
         <v>12</v>
@@ -1987,25 +1985,23 @@
         <v>2.6</v>
       </c>
       <c r="Y13" t="n">
-        <v>337.9</v>
+        <v>337.4</v>
       </c>
       <c r="Z13" t="n">
-        <v>12.7</v>
-      </c>
-      <c r="AA13" t="n">
-        <v>21.9</v>
-      </c>
+        <v>8.199999999999999</v>
+      </c>
+      <c r="AA13" t="inlineStr"/>
       <c r="AB13" t="n">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="AC13" t="n">
-        <v>3.4</v>
+        <v>0.5</v>
       </c>
       <c r="AD13" t="n">
-        <v>3.2</v>
+        <v>2.8</v>
       </c>
       <c r="AE13" t="n">
-        <v>7.8</v>
+        <v>2.7</v>
       </c>
       <c r="AF13" t="n">
         <v>23256</v>
@@ -2320,7 +2316,7 @@
         <v>356.1</v>
       </c>
       <c r="O16" t="n">
-        <v>13.7</v>
+        <v>13.5</v>
       </c>
       <c r="P16" t="n">
         <v>18.47</v>
@@ -2350,25 +2346,25 @@
         <v>6.8</v>
       </c>
       <c r="Y16" t="n">
-        <v>356.3</v>
+        <v>356.2</v>
       </c>
       <c r="Z16" t="n">
-        <v>13.3</v>
+        <v>13</v>
       </c>
       <c r="AA16" t="n">
         <v>24.4</v>
       </c>
       <c r="AB16" t="n">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="AC16" t="n">
-        <v>2.9</v>
+        <v>0.8</v>
       </c>
       <c r="AD16" t="n">
-        <v>15.4</v>
+        <v>15</v>
       </c>
       <c r="AE16" t="n">
-        <v>9.800000000000001</v>
+        <v>4.1</v>
       </c>
       <c r="AF16" t="n">
         <v>38796.7</v>
@@ -2446,10 +2442,10 @@
         <v>3.1</v>
       </c>
       <c r="N17" t="n">
-        <v>358.9</v>
+        <v>358.7</v>
       </c>
       <c r="O17" t="n">
-        <v>16.1</v>
+        <v>14.9</v>
       </c>
       <c r="P17" t="n">
         <v>24.47</v>
@@ -2479,25 +2475,25 @@
         <v>7.4</v>
       </c>
       <c r="Y17" t="n">
-        <v>360.5</v>
+        <v>360.3</v>
       </c>
       <c r="Z17" t="n">
-        <v>15.9</v>
+        <v>14.5</v>
       </c>
       <c r="AA17" t="n">
         <v>-20.2</v>
       </c>
       <c r="AB17" t="n">
-        <v>2.3</v>
+        <v>2.2</v>
       </c>
       <c r="AC17" t="n">
-        <v>4.2</v>
+        <v>1.5</v>
       </c>
       <c r="AD17" t="n">
-        <v>10.1</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="AE17" t="n">
-        <v>9.1</v>
+        <v>5.8</v>
       </c>
       <c r="AF17" t="n">
         <v>43156.2</v>
@@ -2833,10 +2829,10 @@
         <v>0.9</v>
       </c>
       <c r="N20" t="n">
-        <v>312.9</v>
+        <v>312.4</v>
       </c>
       <c r="O20" t="n">
-        <v>15.2</v>
+        <v>10.3</v>
       </c>
       <c r="P20" t="n">
         <v>32.65</v>
@@ -2866,25 +2862,25 @@
         <v>1.4</v>
       </c>
       <c r="Y20" t="n">
-        <v>312.4</v>
+        <v>311.8</v>
       </c>
       <c r="Z20" t="n">
-        <v>16.4</v>
+        <v>10.9</v>
       </c>
       <c r="AA20" t="n">
         <v>3.6</v>
       </c>
       <c r="AB20" t="n">
-        <v>1.2</v>
+        <v>1.1</v>
       </c>
       <c r="AC20" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AD20" t="n">
+        <v>6.9</v>
+      </c>
+      <c r="AE20" t="n">
         <v>1.3</v>
-      </c>
-      <c r="AD20" t="n">
-        <v>7</v>
-      </c>
-      <c r="AE20" t="n">
-        <v>2.3</v>
       </c>
       <c r="AF20" t="n">
         <v>18710.6</v>
@@ -2962,10 +2958,10 @@
         <v>1.5</v>
       </c>
       <c r="N21" t="n">
-        <v>393.3</v>
+        <v>393.1</v>
       </c>
       <c r="O21" t="n">
-        <v>21.8</v>
+        <v>20.9</v>
       </c>
       <c r="P21" t="n">
         <v>26.42</v>
@@ -2995,10 +2991,10 @@
         <v>4.6</v>
       </c>
       <c r="Y21" t="n">
-        <v>388.6</v>
+        <v>388.3</v>
       </c>
       <c r="Z21" t="n">
-        <v>20.9</v>
+        <v>19.6</v>
       </c>
       <c r="AA21" t="n">
         <v>14.7</v>
@@ -3007,13 +3003,13 @@
         <v>1.8</v>
       </c>
       <c r="AC21" t="n">
-        <v>2.4</v>
+        <v>1.2</v>
       </c>
       <c r="AD21" t="n">
-        <v>7.2</v>
+        <v>7</v>
       </c>
       <c r="AE21" t="n">
-        <v>5.7</v>
+        <v>4.6</v>
       </c>
       <c r="AF21" t="n">
         <v>25666.8</v>
@@ -3091,10 +3087,10 @@
         <v>2.4</v>
       </c>
       <c r="N22" t="n">
-        <v>318</v>
+        <v>317.8</v>
       </c>
       <c r="O22" t="n">
-        <v>16.8</v>
+        <v>15.6</v>
       </c>
       <c r="P22" t="n">
         <v>22.8</v>
@@ -3124,25 +3120,25 @@
         <v>4.8</v>
       </c>
       <c r="Y22" t="n">
-        <v>316.5</v>
+        <v>316.3</v>
       </c>
       <c r="Z22" t="n">
-        <v>16.8</v>
+        <v>15.5</v>
       </c>
       <c r="AA22" t="n">
         <v>-0.6</v>
       </c>
       <c r="AB22" t="n">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="AC22" t="n">
-        <v>1.4</v>
+        <v>1.2</v>
       </c>
       <c r="AD22" t="n">
-        <v>11.7</v>
+        <v>11.6</v>
       </c>
       <c r="AE22" t="n">
-        <v>7.5</v>
+        <v>7.3</v>
       </c>
       <c r="AF22" t="n">
         <v>17449.2</v>
@@ -3742,16 +3738,16 @@
         <v>-6.6</v>
       </c>
       <c r="AB27" t="n">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="AC27" t="n">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="AD27" t="n">
-        <v>7.9</v>
+        <v>7.8</v>
       </c>
       <c r="AE27" t="n">
-        <v>3.2</v>
+        <v>2</v>
       </c>
       <c r="AF27" t="n">
         <v>34533.3</v>
@@ -3817,10 +3813,10 @@
         <v>1</v>
       </c>
       <c r="N28" t="n">
-        <v>275.6</v>
+        <v>275.3</v>
       </c>
       <c r="O28" t="n">
-        <v>17</v>
+        <v>12.4</v>
       </c>
       <c r="P28" t="n">
         <v>33.35</v>
@@ -3850,10 +3846,10 @@
         <v>1.6</v>
       </c>
       <c r="Y28" t="n">
-        <v>270.6</v>
+        <v>270.1</v>
       </c>
       <c r="Z28" t="n">
-        <v>17.6</v>
+        <v>10.4</v>
       </c>
       <c r="AA28" t="n">
         <v>10.6</v>
@@ -3862,13 +3858,13 @@
         <v>1.8</v>
       </c>
       <c r="AC28" t="n">
-        <v>1.4</v>
+        <v>0.5</v>
       </c>
       <c r="AD28" t="n">
-        <v>14.6</v>
+        <v>14.5</v>
       </c>
       <c r="AE28" t="n">
-        <v>5</v>
+        <v>3.9</v>
       </c>
       <c r="AF28" t="n">
         <v>13324.6</v>
@@ -3946,10 +3942,10 @@
         <v>0.7</v>
       </c>
       <c r="N29" t="n">
-        <v>287.1</v>
+        <v>286.9</v>
       </c>
       <c r="O29" t="n">
-        <v>10.6</v>
+        <v>10</v>
       </c>
       <c r="P29" t="n">
         <v>32.88</v>
@@ -3979,10 +3975,10 @@
         <v>3.2</v>
       </c>
       <c r="Y29" t="n">
-        <v>286.2</v>
+        <v>286</v>
       </c>
       <c r="Z29" t="n">
-        <v>10.3</v>
+        <v>9.6</v>
       </c>
       <c r="AA29" t="n">
         <v>4.1</v>
@@ -3991,13 +3987,13 @@
         <v>1.2</v>
       </c>
       <c r="AC29" t="n">
-        <v>1.6</v>
+        <v>0.2</v>
       </c>
       <c r="AD29" t="n">
-        <v>8.699999999999999</v>
+        <v>8.5</v>
       </c>
       <c r="AE29" t="n">
-        <v>6</v>
+        <v>1.7</v>
       </c>
       <c r="AF29" t="n">
         <v>24370.7</v>
@@ -4120,13 +4116,13 @@
         <v>1.4</v>
       </c>
       <c r="AC30" t="n">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="AD30" t="n">
         <v>6.4</v>
       </c>
       <c r="AE30" t="n">
-        <v>4</v>
+        <v>3.9</v>
       </c>
       <c r="AF30" t="n">
         <v>34566.6</v>
@@ -4336,7 +4332,7 @@
         <v>646.6</v>
       </c>
       <c r="O32" t="n">
-        <v>82.7</v>
+        <v>82.8</v>
       </c>
       <c r="P32" t="n">
         <v>28.82</v>
@@ -4393,10 +4389,10 @@
         <v>24088.3</v>
       </c>
       <c r="AH32" t="n">
-        <v>733.2</v>
+        <v>734</v>
       </c>
       <c r="AI32" t="n">
-        <v>19.7</v>
+        <v>18.1</v>
       </c>
       <c r="AJ32" t="n">
         <v>10.6</v>
@@ -4405,7 +4401,7 @@
         <v>2.5</v>
       </c>
       <c r="AL32" t="n">
-        <v>9.5</v>
+        <v>9.6</v>
       </c>
       <c r="AM32" t="n">
         <v>2.4</v>
@@ -4462,10 +4458,10 @@
         <v>1.7</v>
       </c>
       <c r="N33" t="n">
-        <v>418.5</v>
+        <v>418.3</v>
       </c>
       <c r="O33" t="n">
-        <v>18.1</v>
+        <v>17.7</v>
       </c>
       <c r="P33" t="n">
         <v>16.6</v>
@@ -4495,25 +4491,25 @@
         <v>2</v>
       </c>
       <c r="Y33" t="n">
-        <v>411.2</v>
+        <v>410.9</v>
       </c>
       <c r="Z33" t="n">
-        <v>14.4</v>
+        <v>13.4</v>
       </c>
       <c r="AA33" t="n">
         <v>4.7</v>
       </c>
       <c r="AB33" t="n">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="AC33" t="n">
-        <v>2.2</v>
+        <v>0.9</v>
       </c>
       <c r="AD33" t="n">
-        <v>10.5</v>
+        <v>10.2</v>
       </c>
       <c r="AE33" t="n">
-        <v>5.2</v>
+        <v>2.6</v>
       </c>
       <c r="AF33" t="n">
         <v>26652.8</v>
@@ -5020,16 +5016,16 @@
         <v>30.1</v>
       </c>
       <c r="AB37" t="n">
-        <v>4.2</v>
+        <v>4.1</v>
       </c>
       <c r="AC37" t="n">
-        <v>3</v>
+        <v>2.7</v>
       </c>
       <c r="AD37" t="n">
-        <v>8.1</v>
+        <v>8</v>
       </c>
       <c r="AE37" t="n">
-        <v>5.3</v>
+        <v>4.8</v>
       </c>
       <c r="AF37" t="n">
         <v>48512.5</v>
@@ -5641,16 +5637,16 @@
         <v>28.1</v>
       </c>
       <c r="AB42" t="n">
-        <v>1.6</v>
+        <v>1.5</v>
       </c>
       <c r="AC42" t="n">
-        <v>1.5</v>
+        <v>0.6</v>
       </c>
       <c r="AD42" t="n">
-        <v>7.8</v>
+        <v>7.6</v>
       </c>
       <c r="AE42" t="n">
-        <v>5.2</v>
+        <v>2.6</v>
       </c>
       <c r="AF42" t="n">
         <v>23467.5</v>
@@ -5857,10 +5853,10 @@
         <v>1.3</v>
       </c>
       <c r="N44" t="n">
-        <v>348.4</v>
+        <v>347.9</v>
       </c>
       <c r="O44" t="n">
-        <v>29</v>
+        <v>26.8</v>
       </c>
       <c r="P44" t="n">
         <v>35.52</v>
@@ -5890,25 +5886,25 @@
         <v>2.6</v>
       </c>
       <c r="Y44" t="n">
-        <v>343.6</v>
+        <v>343.3</v>
       </c>
       <c r="Z44" t="n">
-        <v>24.9</v>
+        <v>23.9</v>
       </c>
       <c r="AA44" t="n">
         <v>36.4</v>
       </c>
       <c r="AB44" t="n">
-        <v>1.6</v>
+        <v>1.5</v>
       </c>
       <c r="AC44" t="n">
-        <v>1.9</v>
+        <v>0.5</v>
       </c>
       <c r="AD44" t="n">
-        <v>7.9</v>
+        <v>7.7</v>
       </c>
       <c r="AE44" t="n">
-        <v>5.3</v>
+        <v>2.1</v>
       </c>
       <c r="AF44" t="n">
         <v>25282.2</v>
@@ -5917,10 +5913,10 @@
         <v>12435.5</v>
       </c>
       <c r="AH44" t="n">
-        <v>393.5</v>
+        <v>391.1</v>
       </c>
       <c r="AI44" t="n">
-        <v>25.3</v>
+        <v>5.6</v>
       </c>
       <c r="AJ44" t="n">
         <v>11.9</v>
@@ -5929,10 +5925,10 @@
         <v>2.2</v>
       </c>
       <c r="AL44" t="n">
-        <v>3.1</v>
+        <v>3</v>
       </c>
       <c r="AM44" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="45">
@@ -6019,7 +6015,7 @@
         <v>3.4</v>
       </c>
       <c r="Y45" t="n">
-        <v>461.3</v>
+        <v>461.2</v>
       </c>
       <c r="Z45" t="n">
         <v>50.5</v>
@@ -6031,13 +6027,13 @@
         <v>0.6</v>
       </c>
       <c r="AC45" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AD45" t="n">
         <v>1.6</v>
       </c>
-      <c r="AD45" t="n">
-        <v>1.7</v>
-      </c>
       <c r="AE45" t="n">
-        <v>3.3</v>
+        <v>0.7</v>
       </c>
       <c r="AF45" t="n">
         <v>50462.1</v>
@@ -6115,10 +6111,10 @@
         <v>2.1</v>
       </c>
       <c r="N46" t="n">
-        <v>348.3</v>
+        <v>348</v>
       </c>
       <c r="O46" t="n">
-        <v>26.6</v>
+        <v>25.3</v>
       </c>
       <c r="P46" t="n">
         <v>62.88</v>
@@ -6148,10 +6144,10 @@
         <v>3.4</v>
       </c>
       <c r="Y46" t="n">
-        <v>344.2</v>
+        <v>343.8</v>
       </c>
       <c r="Z46" t="n">
-        <v>25.6</v>
+        <v>24</v>
       </c>
       <c r="AA46" t="n">
         <v>-9.1</v>
@@ -6160,13 +6156,13 @@
         <v>0.7</v>
       </c>
       <c r="AC46" t="n">
-        <v>1.3</v>
+        <v>0.6</v>
       </c>
       <c r="AD46" t="n">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="AE46" t="n">
-        <v>3.6</v>
+        <v>2.7</v>
       </c>
       <c r="AF46" t="n">
         <v>33627.3</v>
@@ -6244,10 +6240,10 @@
         <v>1.9</v>
       </c>
       <c r="N47" t="n">
-        <v>397.6</v>
+        <v>397.2</v>
       </c>
       <c r="O47" t="n">
-        <v>18.4</v>
+        <v>15.5</v>
       </c>
       <c r="P47" t="n">
         <v>37.17</v>
@@ -6277,25 +6273,25 @@
         <v>2.2</v>
       </c>
       <c r="Y47" t="n">
-        <v>397.6</v>
+        <v>397.2</v>
       </c>
       <c r="Z47" t="n">
-        <v>18.4</v>
+        <v>15.5</v>
       </c>
       <c r="AA47" t="n">
         <v>-1.3</v>
       </c>
       <c r="AB47" t="n">
-        <v>1.1</v>
+        <v>1</v>
       </c>
       <c r="AC47" t="n">
-        <v>2.1</v>
+        <v>0.4</v>
       </c>
       <c r="AD47" t="n">
-        <v>4.1</v>
+        <v>4</v>
       </c>
       <c r="AE47" t="n">
-        <v>2.9</v>
+        <v>1.4</v>
       </c>
       <c r="AF47" t="n">
         <v>31571.1</v>
@@ -6427,16 +6423,16 @@
         <v>8</v>
       </c>
       <c r="AJ48" t="n">
-        <v>7.5</v>
+        <v>5.6</v>
       </c>
       <c r="AK48" t="n">
-        <v>18.7</v>
+        <v>0.5</v>
       </c>
       <c r="AL48" t="n">
-        <v>1.6</v>
+        <v>1.1</v>
       </c>
       <c r="AM48" t="n">
-        <v>5.1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="49">
@@ -6490,10 +6486,10 @@
         <v>1</v>
       </c>
       <c r="N49" t="n">
-        <v>510.2</v>
+        <v>509.6</v>
       </c>
       <c r="O49" t="n">
-        <v>30.2</v>
+        <v>26.4</v>
       </c>
       <c r="P49" t="n">
         <v>17.28</v>
@@ -6523,25 +6519,25 @@
         <v>4.9</v>
       </c>
       <c r="Y49" t="n">
-        <v>518.9</v>
+        <v>518.3</v>
       </c>
       <c r="Z49" t="n">
-        <v>27.7</v>
+        <v>22.3</v>
       </c>
       <c r="AA49" t="n">
         <v>-31.5</v>
       </c>
       <c r="AB49" t="n">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="AC49" t="n">
-        <v>3.7</v>
+        <v>0.9</v>
       </c>
       <c r="AD49" t="n">
-        <v>6.7</v>
+        <v>6.6</v>
       </c>
       <c r="AE49" t="n">
-        <v>3.2</v>
+        <v>2.4</v>
       </c>
       <c r="AF49" t="n">
         <v>41410.6</v>
@@ -6619,10 +6615,10 @@
         <v>6.1</v>
       </c>
       <c r="N50" t="n">
-        <v>504.8</v>
+        <v>504.9</v>
       </c>
       <c r="O50" t="n">
-        <v>29.6</v>
+        <v>29.3</v>
       </c>
       <c r="P50" t="n">
         <v>17.03</v>
@@ -6661,16 +6657,16 @@
         <v>24.5</v>
       </c>
       <c r="AB50" t="n">
-        <v>6.9</v>
+        <v>6.8</v>
       </c>
       <c r="AC50" t="n">
-        <v>7.6</v>
+        <v>7.5</v>
       </c>
       <c r="AD50" t="n">
-        <v>15.4</v>
+        <v>15.2</v>
       </c>
       <c r="AE50" t="n">
-        <v>17</v>
+        <v>16.8</v>
       </c>
       <c r="AF50" t="n">
         <v>54129.6</v>
@@ -6679,22 +6675,22 @@
         <v>22038.3</v>
       </c>
       <c r="AH50" t="n">
-        <v>477.8</v>
+        <v>478.3</v>
       </c>
       <c r="AI50" t="n">
-        <v>30.1</v>
+        <v>29.7</v>
       </c>
       <c r="AJ50" t="n">
-        <v>35.6</v>
+        <v>34.6</v>
       </c>
       <c r="AK50" t="n">
-        <v>13.9</v>
+        <v>8.6</v>
       </c>
       <c r="AL50" t="n">
-        <v>13.5</v>
+        <v>13.2</v>
       </c>
       <c r="AM50" t="n">
-        <v>4.7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51">
@@ -6751,7 +6747,7 @@
         <v>435.2</v>
       </c>
       <c r="O51" t="n">
-        <v>40.2</v>
+        <v>40.1</v>
       </c>
       <c r="P51" t="n">
         <v>49.93</v>
@@ -6784,7 +6780,7 @@
         <v>428.6</v>
       </c>
       <c r="Z51" t="n">
-        <v>31.2</v>
+        <v>31</v>
       </c>
       <c r="AA51" t="n">
         <v>66.3</v>
@@ -6793,13 +6789,13 @@
         <v>1.5</v>
       </c>
       <c r="AC51" t="n">
-        <v>1.7</v>
+        <v>0.7</v>
       </c>
       <c r="AD51" t="n">
-        <v>4.6</v>
+        <v>4.5</v>
       </c>
       <c r="AE51" t="n">
-        <v>3.4</v>
+        <v>1.6</v>
       </c>
       <c r="AF51" t="n">
         <v>54864.6</v>
@@ -7006,10 +7002,10 @@
         <v>0.7</v>
       </c>
       <c r="N53" t="n">
-        <v>391.5</v>
+        <v>391.4</v>
       </c>
       <c r="O53" t="n">
-        <v>19.6</v>
+        <v>19.3</v>
       </c>
       <c r="P53" t="n">
         <v>24</v>
@@ -7039,16 +7035,16 @@
         <v>2.4</v>
       </c>
       <c r="Y53" t="n">
-        <v>391.5</v>
+        <v>391.4</v>
       </c>
       <c r="Z53" t="n">
-        <v>19.6</v>
+        <v>19.3</v>
       </c>
       <c r="AA53" t="n">
         <v>1.8</v>
       </c>
       <c r="AB53" t="n">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="AC53" t="n">
         <v>0.2</v>
@@ -7252,10 +7248,10 @@
         <v>2.1</v>
       </c>
       <c r="N55" t="n">
-        <v>403.5</v>
+        <v>403.1</v>
       </c>
       <c r="O55" t="n">
-        <v>37.8</v>
+        <v>36.9</v>
       </c>
       <c r="P55" t="n">
         <v>40.17</v>
@@ -7285,10 +7281,10 @@
         <v>4.8</v>
       </c>
       <c r="Y55" t="n">
-        <v>399.3</v>
+        <v>398.9</v>
       </c>
       <c r="Z55" t="n">
-        <v>35.8</v>
+        <v>34.7</v>
       </c>
       <c r="AA55" t="n">
         <v>41.5</v>
@@ -7381,10 +7377,10 @@
         <v>6.1</v>
       </c>
       <c r="N56" t="n">
-        <v>487.9</v>
+        <v>487.5</v>
       </c>
       <c r="O56" t="n">
-        <v>36.4</v>
+        <v>35.3</v>
       </c>
       <c r="P56" t="n">
         <v>23.17</v>
@@ -7441,10 +7437,10 @@
         <v>70318.8</v>
       </c>
       <c r="AH56" t="n">
-        <v>504</v>
+        <v>502.6</v>
       </c>
       <c r="AI56" t="n">
-        <v>20.5</v>
+        <v>10.5</v>
       </c>
       <c r="AJ56" t="n">
         <v>26.7</v>
@@ -7453,10 +7449,10 @@
         <v>3.2</v>
       </c>
       <c r="AL56" t="n">
-        <v>11.4</v>
+        <v>11.3</v>
       </c>
       <c r="AM56" t="n">
-        <v>1.8</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="57">
@@ -7951,16 +7947,16 @@
         <v>11.7</v>
       </c>
       <c r="AJ60" t="n">
-        <v>11.3</v>
+        <v>10.8</v>
       </c>
       <c r="AK60" t="n">
-        <v>6.8</v>
+        <v>2.7</v>
       </c>
       <c r="AL60" t="n">
-        <v>2.1</v>
+        <v>2</v>
       </c>
       <c r="AM60" t="n">
-        <v>1.3</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="61">
@@ -8014,10 +8010,10 @@
         <v>1.2</v>
       </c>
       <c r="N61" t="n">
-        <v>380.1</v>
+        <v>379.5</v>
       </c>
       <c r="O61" t="n">
-        <v>20.7</v>
+        <v>13</v>
       </c>
       <c r="P61" t="n">
         <v>26.02</v>
@@ -8047,25 +8043,25 @@
         <v>1.4</v>
       </c>
       <c r="Y61" t="n">
-        <v>380.1</v>
+        <v>379.5</v>
       </c>
       <c r="Z61" t="n">
-        <v>20.7</v>
+        <v>13</v>
       </c>
       <c r="AA61" t="n">
         <v>3.7</v>
       </c>
       <c r="AB61" t="n">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="AC61" t="n">
-        <v>1.3</v>
+        <v>0.4</v>
       </c>
       <c r="AD61" t="n">
         <v>2.5</v>
       </c>
       <c r="AE61" t="n">
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="AF61" t="n">
         <v>75110</v>
@@ -8131,10 +8127,10 @@
         <v>3.4</v>
       </c>
       <c r="N62" t="n">
-        <v>440.9</v>
+        <v>440</v>
       </c>
       <c r="O62" t="n">
-        <v>28.5</v>
+        <v>23.9</v>
       </c>
       <c r="P62" t="n">
         <v>22.32</v>
@@ -8191,22 +8187,22 @@
         <v>30432.3</v>
       </c>
       <c r="AH62" t="n">
-        <v>450.1</v>
+        <v>448.6</v>
       </c>
       <c r="AI62" t="n">
-        <v>36.3</v>
+        <v>29.4</v>
       </c>
       <c r="AJ62" t="n">
-        <v>10.1</v>
+        <v>10</v>
       </c>
       <c r="AK62" t="n">
-        <v>5.3</v>
+        <v>4.7</v>
       </c>
       <c r="AL62" t="n">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="AM62" t="n">
-        <v>3</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="63">
@@ -8305,13 +8301,13 @@
         <v>2.6</v>
       </c>
       <c r="AC63" t="n">
-        <v>2.1</v>
+        <v>2</v>
       </c>
       <c r="AD63" t="n">
-        <v>14.1</v>
+        <v>14</v>
       </c>
       <c r="AE63" t="n">
-        <v>7.3</v>
+        <v>7.2</v>
       </c>
       <c r="AF63" t="n">
         <v>26441</v>
@@ -8389,10 +8385,10 @@
         <v>5</v>
       </c>
       <c r="N64" t="n">
-        <v>413.7</v>
+        <v>413.4</v>
       </c>
       <c r="O64" t="n">
-        <v>20</v>
+        <v>17.9</v>
       </c>
       <c r="P64" t="n">
         <v>6.58</v>
@@ -8422,25 +8418,25 @@
         <v>3</v>
       </c>
       <c r="Y64" t="n">
-        <v>409.9</v>
+        <v>409.2</v>
       </c>
       <c r="Z64" t="n">
-        <v>15.7</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="AA64" t="n">
         <v>9.300000000000001</v>
       </c>
       <c r="AB64" t="n">
-        <v>7.5</v>
+        <v>7.1</v>
       </c>
       <c r="AC64" t="n">
-        <v>5.8</v>
+        <v>2.6</v>
       </c>
       <c r="AD64" t="n">
-        <v>26.3</v>
+        <v>25.3</v>
       </c>
       <c r="AE64" t="n">
-        <v>12.2</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="AF64" t="n">
         <v>76677.7</v>
@@ -8455,16 +8451,16 @@
         <v>23.3</v>
       </c>
       <c r="AJ64" t="n">
-        <v>40.3</v>
+        <v>40.2</v>
       </c>
       <c r="AK64" t="n">
-        <v>15.9</v>
+        <v>16</v>
       </c>
       <c r="AL64" t="n">
         <v>11.7</v>
       </c>
       <c r="AM64" t="n">
-        <v>4.4</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="65">
@@ -8647,10 +8643,10 @@
         <v>3</v>
       </c>
       <c r="N66" t="n">
-        <v>449.1</v>
+        <v>448.9</v>
       </c>
       <c r="O66" t="n">
-        <v>24.9</v>
+        <v>23.8</v>
       </c>
       <c r="P66" t="n">
         <v>59.77</v>
@@ -8680,25 +8676,25 @@
         <v>5.7</v>
       </c>
       <c r="Y66" t="n">
-        <v>443.1</v>
+        <v>442.8</v>
       </c>
       <c r="Z66" t="n">
-        <v>24</v>
+        <v>22.4</v>
       </c>
       <c r="AA66" t="n">
         <v>19</v>
       </c>
       <c r="AB66" t="n">
-        <v>2.2</v>
+        <v>2.1</v>
       </c>
       <c r="AC66" t="n">
-        <v>2.2</v>
+        <v>0.8</v>
       </c>
       <c r="AD66" t="n">
-        <v>6.6</v>
+        <v>6.4</v>
       </c>
       <c r="AE66" t="n">
-        <v>4.3</v>
+        <v>2.5</v>
       </c>
       <c r="AF66" t="n">
         <v>43371.6</v>
@@ -8776,10 +8772,10 @@
         <v>5.9</v>
       </c>
       <c r="N67" t="n">
-        <v>588.9</v>
+        <v>587.6</v>
       </c>
       <c r="O67" t="n">
-        <v>100.1</v>
+        <v>98.90000000000001</v>
       </c>
       <c r="P67" t="n">
         <v>59.52</v>
@@ -8809,10 +8805,10 @@
         <v>5.2</v>
       </c>
       <c r="Y67" t="n">
-        <v>573.3</v>
+        <v>572.5</v>
       </c>
       <c r="Z67" t="n">
-        <v>97.40000000000001</v>
+        <v>96.5</v>
       </c>
       <c r="AA67" t="n">
         <v>95.8</v>
@@ -8821,7 +8817,7 @@
         <v>1.5</v>
       </c>
       <c r="AC67" t="n">
-        <v>1.6</v>
+        <v>1.5</v>
       </c>
       <c r="AD67" t="n">
         <v>2.5</v>
@@ -8830,16 +8826,16 @@
         <v>1.9</v>
       </c>
       <c r="AF67" t="n">
-        <v>133933.3</v>
+        <v>101504</v>
       </c>
       <c r="AG67" t="n">
-        <v>340786.5</v>
+        <v>266209.8</v>
       </c>
       <c r="AH67" t="n">
-        <v>686.8</v>
+        <v>685.1</v>
       </c>
       <c r="AI67" t="n">
-        <v>46.6</v>
+        <v>42.2</v>
       </c>
       <c r="AJ67" t="n">
         <v>12</v>
@@ -8848,10 +8844,10 @@
         <v>4.3</v>
       </c>
       <c r="AL67" t="n">
-        <v>9.6</v>
+        <v>9.5</v>
       </c>
       <c r="AM67" t="n">
-        <v>4.4</v>
+        <v>4.1</v>
       </c>
     </row>
     <row r="68">
@@ -8905,10 +8901,10 @@
         <v>4</v>
       </c>
       <c r="N68" t="n">
-        <v>602.2</v>
+        <v>602</v>
       </c>
       <c r="O68" t="n">
-        <v>78.90000000000001</v>
+        <v>78.40000000000001</v>
       </c>
       <c r="P68" t="n">
         <v>34.55</v>
@@ -8938,31 +8934,31 @@
         <v>2.9</v>
       </c>
       <c r="Y68" t="n">
-        <v>625</v>
+        <v>624.9</v>
       </c>
       <c r="Z68" t="n">
-        <v>66.3</v>
+        <v>65.5</v>
       </c>
       <c r="AA68" t="n">
         <v>-2.4</v>
       </c>
       <c r="AB68" t="n">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="AC68" t="n">
-        <v>1.6</v>
+        <v>0.7</v>
       </c>
       <c r="AD68" t="n">
         <v>1</v>
       </c>
       <c r="AE68" t="n">
-        <v>1.6</v>
+        <v>0.8</v>
       </c>
       <c r="AF68" t="n">
-        <v>155850.2</v>
+        <v>134641.6</v>
       </c>
       <c r="AG68" t="n">
-        <v>264483.8</v>
+        <v>198892.9</v>
       </c>
       <c r="AH68" t="n">
         <v>494.3</v>
@@ -9088,10 +9084,10 @@
         <v>1.8</v>
       </c>
       <c r="AF69" t="n">
-        <v>117130.5</v>
+        <v>114308.2</v>
       </c>
       <c r="AG69" t="n">
-        <v>97740.60000000001</v>
+        <v>91110.8</v>
       </c>
       <c r="AH69" t="n">
         <v>711.1</v>
@@ -9163,10 +9159,10 @@
         <v>1.7</v>
       </c>
       <c r="N70" t="n">
-        <v>342.3</v>
+        <v>341.8</v>
       </c>
       <c r="O70" t="n">
-        <v>17.5</v>
+        <v>13</v>
       </c>
       <c r="P70" t="n">
         <v>25.92</v>
@@ -9196,25 +9192,25 @@
         <v>5.1</v>
       </c>
       <c r="Y70" t="n">
-        <v>341.6</v>
+        <v>341.1</v>
       </c>
       <c r="Z70" t="n">
-        <v>19.2</v>
+        <v>14.1</v>
       </c>
       <c r="AA70" t="n">
         <v>9.6</v>
       </c>
       <c r="AB70" t="n">
-        <v>2.1</v>
+        <v>1.8</v>
       </c>
       <c r="AC70" t="n">
-        <v>6.7</v>
+        <v>0.4</v>
       </c>
       <c r="AD70" t="n">
-        <v>10.1</v>
+        <v>9.4</v>
       </c>
       <c r="AE70" t="n">
-        <v>14.4</v>
+        <v>2.4</v>
       </c>
       <c r="AF70" t="n">
         <v>33504</v>
@@ -9604,10 +9600,10 @@
         <v>7.5</v>
       </c>
       <c r="AJ73" t="n">
-        <v>14.9</v>
+        <v>14.8</v>
       </c>
       <c r="AK73" t="n">
-        <v>4.5</v>
+        <v>4.3</v>
       </c>
       <c r="AL73" t="n">
         <v>2.2</v>
@@ -9965,16 +9961,16 @@
         <v>45.3</v>
       </c>
       <c r="AB76" t="n">
-        <v>8.5</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="AC76" t="n">
-        <v>6.3</v>
+        <v>5.6</v>
       </c>
       <c r="AD76" t="n">
-        <v>23.6</v>
+        <v>23</v>
       </c>
       <c r="AE76" t="n">
-        <v>13.8</v>
+        <v>12.1</v>
       </c>
       <c r="AF76" t="n">
         <v>64359.9</v>
@@ -9989,16 +9985,16 @@
         <v>35.7</v>
       </c>
       <c r="AJ76" t="n">
-        <v>20.2</v>
+        <v>19.3</v>
       </c>
       <c r="AK76" t="n">
-        <v>17.8</v>
+        <v>15.3</v>
       </c>
       <c r="AL76" t="n">
-        <v>6.8</v>
+        <v>6.4</v>
       </c>
       <c r="AM76" t="n">
-        <v>8.4</v>
+        <v>7.3</v>
       </c>
     </row>
     <row r="77">
@@ -10052,10 +10048,10 @@
         <v>2.6</v>
       </c>
       <c r="N77" t="n">
-        <v>415.5</v>
+        <v>415.1</v>
       </c>
       <c r="O77" t="n">
-        <v>23.2</v>
+        <v>20.8</v>
       </c>
       <c r="P77" t="n">
         <v>41.73</v>
@@ -10085,25 +10081,25 @@
         <v>6.7</v>
       </c>
       <c r="Y77" t="n">
-        <v>416.5</v>
+        <v>416.1</v>
       </c>
       <c r="Z77" t="n">
-        <v>24.3</v>
+        <v>21.7</v>
       </c>
       <c r="AA77" t="n">
         <v>-11</v>
       </c>
       <c r="AB77" t="n">
-        <v>2.3</v>
+        <v>2.2</v>
       </c>
       <c r="AC77" t="n">
-        <v>2.7</v>
+        <v>1.3</v>
       </c>
       <c r="AD77" t="n">
-        <v>7.7</v>
+        <v>7.5</v>
       </c>
       <c r="AE77" t="n">
-        <v>5.4</v>
+        <v>4.1</v>
       </c>
       <c r="AF77" t="n">
         <v>34782.9</v>
@@ -10181,10 +10177,10 @@
         <v>6</v>
       </c>
       <c r="N78" t="n">
-        <v>517</v>
+        <v>516.5</v>
       </c>
       <c r="O78" t="n">
-        <v>82.2</v>
+        <v>80.7</v>
       </c>
       <c r="P78" t="n">
         <v>45.13</v>
@@ -10214,37 +10210,35 @@
         <v>6.5</v>
       </c>
       <c r="Y78" t="n">
-        <v>491.4</v>
+        <v>490.6</v>
       </c>
       <c r="Z78" t="n">
-        <v>70.59999999999999</v>
-      </c>
-      <c r="AA78" t="n">
-        <v>91.5</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="AA78" t="inlineStr"/>
       <c r="AB78" t="n">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="AC78" t="n">
-        <v>2.3</v>
+        <v>1.2</v>
       </c>
       <c r="AD78" t="n">
         <v>1.9</v>
       </c>
       <c r="AE78" t="n">
-        <v>2.6</v>
+        <v>2.1</v>
       </c>
       <c r="AF78" t="n">
-        <v>48422.6</v>
+        <v>47512.9</v>
       </c>
       <c r="AG78" t="n">
-        <v>45047.6</v>
+        <v>37745.2</v>
       </c>
       <c r="AH78" t="n">
-        <v>614.8</v>
+        <v>615.2</v>
       </c>
       <c r="AI78" t="n">
-        <v>38</v>
+        <v>37.4</v>
       </c>
       <c r="AJ78" t="n">
         <v>16.4</v>
@@ -10376,16 +10370,16 @@
         <v>6.9</v>
       </c>
       <c r="AJ79" t="n">
-        <v>12.6</v>
+        <v>12.3</v>
       </c>
       <c r="AK79" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AL79" t="n">
-        <v>2.8</v>
+        <v>2.7</v>
       </c>
       <c r="AM79" t="n">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="80">
@@ -10685,10 +10679,10 @@
         <v>0.8</v>
       </c>
       <c r="N82" t="n">
-        <v>317.1</v>
+        <v>317</v>
       </c>
       <c r="O82" t="n">
-        <v>10.3</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="P82" t="n">
         <v>52.18</v>
@@ -10718,25 +10712,23 @@
         <v>2.3</v>
       </c>
       <c r="Y82" t="n">
-        <v>317.1</v>
+        <v>317</v>
       </c>
       <c r="Z82" t="n">
-        <v>10.3</v>
-      </c>
-      <c r="AA82" t="n">
-        <v>-45.1</v>
-      </c>
+        <v>9.300000000000001</v>
+      </c>
+      <c r="AA82" t="inlineStr"/>
       <c r="AB82" t="n">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="AC82" t="n">
-        <v>1.2</v>
+        <v>0.5</v>
       </c>
       <c r="AD82" t="n">
-        <v>7.5</v>
+        <v>7.4</v>
       </c>
       <c r="AE82" t="n">
-        <v>4.2</v>
+        <v>3.4</v>
       </c>
       <c r="AF82" t="n">
         <v>19335.1</v>
@@ -10931,10 +10923,10 @@
         <v>1.5</v>
       </c>
       <c r="N84" t="n">
-        <v>426.9</v>
+        <v>426.1</v>
       </c>
       <c r="O84" t="n">
-        <v>22.1</v>
+        <v>20.5</v>
       </c>
       <c r="P84" t="n">
         <v>13.45</v>
@@ -10964,25 +10956,25 @@
         <v>0.9</v>
       </c>
       <c r="Y84" t="n">
-        <v>424.1</v>
+        <v>423.6</v>
       </c>
       <c r="Z84" t="n">
-        <v>20</v>
+        <v>18.5</v>
       </c>
       <c r="AA84" t="n">
         <v>44.3</v>
       </c>
       <c r="AB84" t="n">
-        <v>0.9</v>
+        <v>0.6</v>
       </c>
       <c r="AC84" t="n">
-        <v>4</v>
+        <v>0.4</v>
       </c>
       <c r="AD84" t="n">
-        <v>2.6</v>
+        <v>2.1</v>
       </c>
       <c r="AE84" t="n">
-        <v>7.7</v>
+        <v>1.5</v>
       </c>
       <c r="AF84" t="n">
         <v>28744.9</v>
@@ -10991,10 +10983,10 @@
         <v>16929.1</v>
       </c>
       <c r="AH84" t="n">
-        <v>444.6</v>
+        <v>442.9</v>
       </c>
       <c r="AI84" t="n">
-        <v>26.2</v>
+        <v>24.4</v>
       </c>
       <c r="AJ84" t="n">
         <v>14.2</v>
@@ -11003,7 +10995,7 @@
         <v>6</v>
       </c>
       <c r="AL84" t="n">
-        <v>4.6</v>
+        <v>4.7</v>
       </c>
       <c r="AM84" t="n">
         <v>1.8</v>
@@ -11177,10 +11169,10 @@
         <v>5</v>
       </c>
       <c r="N86" t="n">
-        <v>351.3</v>
+        <v>350.8</v>
       </c>
       <c r="O86" t="n">
-        <v>33</v>
+        <v>32.1</v>
       </c>
       <c r="P86" t="n">
         <v>38.65</v>
@@ -11210,25 +11202,25 @@
         <v>6.5</v>
       </c>
       <c r="Y86" t="n">
-        <v>353.5</v>
+        <v>353</v>
       </c>
       <c r="Z86" t="n">
-        <v>32.1</v>
+        <v>31.1</v>
       </c>
       <c r="AA86" t="n">
         <v>0.6</v>
       </c>
       <c r="AB86" t="n">
-        <v>2.5</v>
+        <v>2.4</v>
       </c>
       <c r="AC86" t="n">
-        <v>2.3</v>
+        <v>1.1</v>
       </c>
       <c r="AD86" t="n">
-        <v>11.5</v>
+        <v>11.3</v>
       </c>
       <c r="AE86" t="n">
-        <v>6.6</v>
+        <v>4.5</v>
       </c>
       <c r="AF86" t="n">
         <v>58556.5</v>
@@ -11306,10 +11298,10 @@
         <v>2.1</v>
       </c>
       <c r="N87" t="n">
-        <v>392</v>
+        <v>391.7</v>
       </c>
       <c r="O87" t="n">
-        <v>28.1</v>
+        <v>26.7</v>
       </c>
       <c r="P87" t="n">
         <v>25.45</v>
@@ -11339,10 +11331,10 @@
         <v>8.4</v>
       </c>
       <c r="Y87" t="n">
-        <v>397.3</v>
+        <v>396.9</v>
       </c>
       <c r="Z87" t="n">
-        <v>29.4</v>
+        <v>27.5</v>
       </c>
       <c r="AA87" t="n">
         <v>17.3</v>
@@ -11438,7 +11430,7 @@
         <v>494.3</v>
       </c>
       <c r="O88" t="n">
-        <v>25.5</v>
+        <v>25.3</v>
       </c>
       <c r="P88" t="n">
         <v>14.75</v>
@@ -11468,10 +11460,10 @@
         <v>5.4</v>
       </c>
       <c r="Y88" t="n">
-        <v>479.9</v>
+        <v>479.8</v>
       </c>
       <c r="Z88" t="n">
-        <v>19</v>
+        <v>18.3</v>
       </c>
       <c r="AA88" t="n">
         <v>25.5</v>
@@ -11480,13 +11472,13 @@
         <v>1</v>
       </c>
       <c r="AC88" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="AD88" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="AE88" t="n">
         <v>1.7</v>
-      </c>
-      <c r="AD88" t="n">
-        <v>2.6</v>
-      </c>
-      <c r="AE88" t="n">
-        <v>3.1</v>
       </c>
       <c r="AF88" t="n">
         <v>55394.1</v>
@@ -11759,10 +11751,10 @@
         <v>28</v>
       </c>
       <c r="AJ90" t="n">
-        <v>22.5</v>
+        <v>22.1</v>
       </c>
       <c r="AK90" t="n">
-        <v>10.4</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="AL90" t="n">
         <v>6.5</v>
@@ -11822,10 +11814,10 @@
         <v>2.1</v>
       </c>
       <c r="N91" t="n">
-        <v>384.3</v>
+        <v>383.5</v>
       </c>
       <c r="O91" t="n">
-        <v>23.9</v>
+        <v>18.5</v>
       </c>
       <c r="P91" t="n">
         <v>23.27</v>
@@ -11882,22 +11874,22 @@
         <v>28131.9</v>
       </c>
       <c r="AH91" t="n">
-        <v>389.6</v>
+        <v>387.6</v>
       </c>
       <c r="AI91" t="n">
-        <v>28.8</v>
+        <v>15.9</v>
       </c>
       <c r="AJ91" t="n">
-        <v>14.8</v>
+        <v>14.3</v>
       </c>
       <c r="AK91" t="n">
-        <v>9.199999999999999</v>
+        <v>5.8</v>
       </c>
       <c r="AL91" t="n">
-        <v>4.1</v>
+        <v>3.6</v>
       </c>
       <c r="AM91" t="n">
-        <v>7.8</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="92">
@@ -11951,10 +11943,10 @@
         <v>2.4</v>
       </c>
       <c r="N92" t="n">
-        <v>395.8</v>
+        <v>394.9</v>
       </c>
       <c r="O92" t="n">
-        <v>23.1</v>
+        <v>16.5</v>
       </c>
       <c r="P92" t="n">
         <v>21.37</v>
@@ -11984,25 +11976,25 @@
         <v>5.8</v>
       </c>
       <c r="Y92" t="n">
-        <v>387.6</v>
+        <v>387.5</v>
       </c>
       <c r="Z92" t="n">
-        <v>16.1</v>
+        <v>15.6</v>
       </c>
       <c r="AA92" t="n">
         <v>-25</v>
       </c>
       <c r="AB92" t="n">
-        <v>1.3</v>
+        <v>1.1</v>
       </c>
       <c r="AC92" t="n">
-        <v>4</v>
+        <v>1.4</v>
       </c>
       <c r="AD92" t="n">
-        <v>4.6</v>
+        <v>4.1</v>
       </c>
       <c r="AE92" t="n">
-        <v>10.7</v>
+        <v>4.7</v>
       </c>
       <c r="AF92" t="n">
         <v>40122.7</v>
@@ -12011,22 +12003,22 @@
         <v>36379</v>
       </c>
       <c r="AH92" t="n">
-        <v>407.6</v>
+        <v>405.8</v>
       </c>
       <c r="AI92" t="n">
+        <v>10.6</v>
+      </c>
+      <c r="AJ92" t="n">
         <v>26.4</v>
       </c>
-      <c r="AJ92" t="n">
-        <v>27.1</v>
-      </c>
       <c r="AK92" t="n">
-        <v>13.8</v>
+        <v>12.1</v>
       </c>
       <c r="AL92" t="n">
-        <v>7.8</v>
+        <v>7.3</v>
       </c>
       <c r="AM92" t="n">
-        <v>7.5</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="93">
@@ -12080,10 +12072,10 @@
         <v>0.9</v>
       </c>
       <c r="N93" t="n">
-        <v>428.1</v>
+        <v>427.5</v>
       </c>
       <c r="O93" t="n">
-        <v>24.5</v>
+        <v>20.9</v>
       </c>
       <c r="P93" t="n">
         <v>16.55</v>
@@ -12113,25 +12105,25 @@
         <v>2</v>
       </c>
       <c r="Y93" t="n">
-        <v>427.1</v>
+        <v>426.5</v>
       </c>
       <c r="Z93" t="n">
-        <v>25.3</v>
+        <v>21.5</v>
       </c>
       <c r="AA93" t="n">
         <v>27.8</v>
       </c>
       <c r="AB93" t="n">
-        <v>1.4</v>
+        <v>1.2</v>
       </c>
       <c r="AC93" t="n">
-        <v>4.4</v>
+        <v>0.6</v>
       </c>
       <c r="AD93" t="n">
-        <v>4.1</v>
+        <v>3.9</v>
       </c>
       <c r="AE93" t="n">
-        <v>5</v>
+        <v>2.1</v>
       </c>
       <c r="AF93" t="n">
         <v>18368</v>
@@ -12338,10 +12330,10 @@
         <v>2.3</v>
       </c>
       <c r="N95" t="n">
-        <v>551.2</v>
+        <v>550.4</v>
       </c>
       <c r="O95" t="n">
-        <v>84.5</v>
+        <v>83.7</v>
       </c>
       <c r="P95" t="n">
         <v>49.92</v>
@@ -12371,16 +12363,16 @@
         <v>3.8</v>
       </c>
       <c r="Y95" t="n">
-        <v>528.7</v>
+        <v>528.1</v>
       </c>
       <c r="Z95" t="n">
-        <v>68.5</v>
+        <v>67.5</v>
       </c>
       <c r="AA95" t="n">
         <v>111</v>
       </c>
       <c r="AB95" t="n">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="AC95" t="n">
         <v>1.1</v>
@@ -12398,7 +12390,7 @@
         <v>38316.1</v>
       </c>
       <c r="AH95" t="n">
-        <v>683.1</v>
+        <v>683.2</v>
       </c>
       <c r="AI95" t="n">
         <v>32.8</v>
@@ -12467,10 +12459,10 @@
         <v>3.2</v>
       </c>
       <c r="N96" t="n">
-        <v>415</v>
+        <v>414.7</v>
       </c>
       <c r="O96" t="n">
-        <v>54.4</v>
+        <v>53.4</v>
       </c>
       <c r="P96" t="n">
         <v>60.48</v>
@@ -12500,23 +12492,23 @@
         <v>3</v>
       </c>
       <c r="Y96" t="n">
-        <v>390.9</v>
+        <v>390.7</v>
       </c>
       <c r="Z96" t="n">
-        <v>34.3</v>
+        <v>32.9</v>
       </c>
       <c r="AA96" t="inlineStr"/>
       <c r="AB96" t="n">
         <v>1</v>
       </c>
       <c r="AC96" t="n">
-        <v>2.8</v>
+        <v>1</v>
       </c>
       <c r="AD96" t="n">
         <v>3.6</v>
       </c>
       <c r="AE96" t="n">
-        <v>3.6</v>
+        <v>2.9</v>
       </c>
       <c r="AF96" t="n">
         <v>22024</v>
@@ -12525,22 +12517,22 @@
         <v>14438</v>
       </c>
       <c r="AH96" t="n">
-        <v>494.9</v>
+        <v>494.4</v>
       </c>
       <c r="AI96" t="n">
-        <v>23.2</v>
+        <v>21.3</v>
       </c>
       <c r="AJ96" t="n">
-        <v>13.6</v>
+        <v>13.5</v>
       </c>
       <c r="AK96" t="n">
-        <v>4.2</v>
+        <v>3.4</v>
       </c>
       <c r="AL96" t="n">
-        <v>5.6</v>
+        <v>5.5</v>
       </c>
       <c r="AM96" t="n">
-        <v>2.2</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="97">
@@ -12850,10 +12842,10 @@
         <v>2.6</v>
       </c>
       <c r="N99" t="n">
-        <v>443.5</v>
+        <v>443.1</v>
       </c>
       <c r="O99" t="n">
-        <v>39.1</v>
+        <v>37.7</v>
       </c>
       <c r="P99" t="n">
         <v>33.62</v>
@@ -12893,13 +12885,13 @@
         <v>1.9</v>
       </c>
       <c r="AC99" t="n">
-        <v>1.3</v>
+        <v>0.9</v>
       </c>
       <c r="AD99" t="n">
-        <v>6.5</v>
+        <v>6.3</v>
       </c>
       <c r="AE99" t="n">
-        <v>4.6</v>
+        <v>3</v>
       </c>
       <c r="AF99" t="n">
         <v>34340.4</v>
@@ -12908,22 +12900,22 @@
         <v>17463.2</v>
       </c>
       <c r="AH99" t="n">
-        <v>488.8</v>
+        <v>487.7</v>
       </c>
       <c r="AI99" t="n">
-        <v>25.4</v>
+        <v>18.5</v>
       </c>
       <c r="AJ99" t="n">
-        <v>5.6</v>
+        <v>5.4</v>
       </c>
       <c r="AK99" t="n">
-        <v>4.8</v>
+        <v>1.3</v>
       </c>
       <c r="AL99" t="n">
-        <v>2.4</v>
+        <v>2.1</v>
       </c>
       <c r="AM99" t="n">
-        <v>5.3</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="100">
@@ -12977,10 +12969,10 @@
         <v>2</v>
       </c>
       <c r="N100" t="n">
-        <v>403.4</v>
+        <v>403.1</v>
       </c>
       <c r="O100" t="n">
-        <v>26.1</v>
+        <v>25.1</v>
       </c>
       <c r="P100" t="n">
         <v>33.6</v>
@@ -13010,10 +13002,10 @@
         <v>5.4</v>
       </c>
       <c r="Y100" t="n">
-        <v>391</v>
+        <v>390.6</v>
       </c>
       <c r="Z100" t="n">
-        <v>17.7</v>
+        <v>15</v>
       </c>
       <c r="AA100" t="n">
         <v>-16.6</v>
@@ -13022,13 +13014,13 @@
         <v>2.1</v>
       </c>
       <c r="AC100" t="n">
-        <v>1.9</v>
+        <v>1.3</v>
       </c>
       <c r="AD100" t="n">
-        <v>8.300000000000001</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="AE100" t="n">
-        <v>5.2</v>
+        <v>4.7</v>
       </c>
       <c r="AF100" t="n">
         <v>25237.6</v>
@@ -13106,10 +13098,10 @@
         <v>2.6</v>
       </c>
       <c r="N101" t="n">
-        <v>344.4</v>
+        <v>344.1</v>
       </c>
       <c r="O101" t="n">
-        <v>23.4</v>
+        <v>22.3</v>
       </c>
       <c r="P101" t="n">
         <v>58.32</v>
@@ -13139,25 +13131,25 @@
         <v>6.6</v>
       </c>
       <c r="Y101" t="n">
-        <v>339.4</v>
+        <v>339</v>
       </c>
       <c r="Z101" t="n">
-        <v>21.5</v>
+        <v>19.9</v>
       </c>
       <c r="AA101" t="n">
         <v>30</v>
       </c>
       <c r="AB101" t="n">
-        <v>1.6</v>
+        <v>1.5</v>
       </c>
       <c r="AC101" t="n">
-        <v>2.4</v>
+        <v>0.8</v>
       </c>
       <c r="AD101" t="n">
-        <v>7.9</v>
+        <v>7.6</v>
       </c>
       <c r="AE101" t="n">
-        <v>6.8</v>
+        <v>3.6</v>
       </c>
       <c r="AF101" t="n">
         <v>28170.3</v>
@@ -13235,10 +13227,10 @@
         <v>2.5</v>
       </c>
       <c r="N102" t="n">
-        <v>423.3</v>
+        <v>423</v>
       </c>
       <c r="O102" t="n">
-        <v>42.7</v>
+        <v>41.9</v>
       </c>
       <c r="P102" t="n">
         <v>51.12</v>
@@ -13268,25 +13260,25 @@
         <v>6.6</v>
       </c>
       <c r="Y102" t="n">
-        <v>420.3</v>
+        <v>420</v>
       </c>
       <c r="Z102" t="n">
-        <v>41.8</v>
+        <v>40.9</v>
       </c>
       <c r="AA102" t="n">
         <v>66.8</v>
       </c>
       <c r="AB102" t="n">
-        <v>1.4</v>
+        <v>1.2</v>
       </c>
       <c r="AC102" t="n">
-        <v>6.2</v>
+        <v>1</v>
       </c>
       <c r="AD102" t="n">
-        <v>4.2</v>
+        <v>4</v>
       </c>
       <c r="AE102" t="n">
-        <v>7</v>
+        <v>2.7</v>
       </c>
       <c r="AF102" t="n">
         <v>35924.5</v>
@@ -13364,10 +13356,10 @@
         <v>0.7</v>
       </c>
       <c r="N103" t="n">
-        <v>506.4</v>
+        <v>505.8</v>
       </c>
       <c r="O103" t="n">
-        <v>39.4</v>
+        <v>37</v>
       </c>
       <c r="P103" t="n">
         <v>12.02</v>
@@ -13424,10 +13416,10 @@
         <v>35676.5</v>
       </c>
       <c r="AH103" t="n">
-        <v>538.5</v>
+        <v>537.1</v>
       </c>
       <c r="AI103" t="n">
-        <v>26.8</v>
+        <v>17.8</v>
       </c>
       <c r="AJ103" t="n">
         <v>2.6</v>
@@ -13493,10 +13485,10 @@
         <v>6.5</v>
       </c>
       <c r="N104" t="n">
-        <v>597.2</v>
+        <v>595.3</v>
       </c>
       <c r="O104" t="n">
-        <v>40.7</v>
+        <v>21.2</v>
       </c>
       <c r="P104" t="n">
         <v>6</v>
@@ -13553,22 +13545,22 @@
         <v>20697.1</v>
       </c>
       <c r="AH104" t="n">
-        <v>598.8</v>
+        <v>596.1</v>
       </c>
       <c r="AI104" t="n">
-        <v>48.6</v>
+        <v>24.7</v>
       </c>
       <c r="AJ104" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AK104" t="n">
-        <v>13.5</v>
+        <v>11.9</v>
       </c>
       <c r="AL104" t="n">
-        <v>10.9</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="AM104" t="n">
-        <v>15.3</v>
+        <v>7.8</v>
       </c>
     </row>
     <row r="105">
@@ -13622,10 +13614,10 @@
         <v>0.3</v>
       </c>
       <c r="N105" t="n">
-        <v>487.7</v>
+        <v>486.7</v>
       </c>
       <c r="O105" t="n">
-        <v>37.6</v>
+        <v>34</v>
       </c>
       <c r="P105" t="n">
         <v>14.87</v>
@@ -13655,23 +13647,23 @@
         <v>2.1</v>
       </c>
       <c r="Y105" t="n">
-        <v>487.7</v>
+        <v>486.7</v>
       </c>
       <c r="Z105" t="n">
-        <v>37.6</v>
+        <v>34</v>
       </c>
       <c r="AA105" t="inlineStr"/>
       <c r="AB105" t="n">
-        <v>0.6</v>
+        <v>0.2</v>
       </c>
       <c r="AC105" t="n">
-        <v>5</v>
+        <v>0.2</v>
       </c>
       <c r="AD105" t="n">
-        <v>1.1</v>
+        <v>0.5</v>
       </c>
       <c r="AE105" t="n">
-        <v>5.8</v>
+        <v>0.4</v>
       </c>
       <c r="AF105" t="n">
         <v>29139.8</v>
@@ -13777,16 +13769,16 @@
       </c>
       <c r="AA106" t="inlineStr"/>
       <c r="AB106" t="n">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="AC106" t="n">
-        <v>2.1</v>
+        <v>0.2</v>
       </c>
       <c r="AD106" t="n">
-        <v>7.6</v>
+        <v>6.9</v>
       </c>
       <c r="AE106" t="n">
-        <v>11</v>
+        <v>1.2</v>
       </c>
       <c r="AF106" t="n">
         <v>64374.6</v>
@@ -14108,10 +14100,10 @@
         <v>1.3</v>
       </c>
       <c r="N109" t="n">
-        <v>452.7</v>
+        <v>452</v>
       </c>
       <c r="O109" t="n">
-        <v>48.6</v>
+        <v>46.7</v>
       </c>
       <c r="P109" t="n">
         <v>46.55</v>
@@ -14168,22 +14160,22 @@
         <v>54589.4</v>
       </c>
       <c r="AH109" t="n">
-        <v>518.8</v>
+        <v>515.9</v>
       </c>
       <c r="AI109" t="n">
-        <v>36.4</v>
+        <v>20.9</v>
       </c>
       <c r="AJ109" t="n">
-        <v>6.3</v>
+        <v>5.7</v>
       </c>
       <c r="AK109" t="n">
-        <v>7.2</v>
+        <v>1.7</v>
       </c>
       <c r="AL109" t="n">
-        <v>3.2</v>
+        <v>2.5</v>
       </c>
       <c r="AM109" t="n">
-        <v>8.300000000000001</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="110">
@@ -14237,10 +14229,10 @@
         <v>0.6</v>
       </c>
       <c r="N110" t="n">
-        <v>586</v>
+        <v>585.7</v>
       </c>
       <c r="O110" t="n">
-        <v>40.4</v>
+        <v>40.1</v>
       </c>
       <c r="P110" t="n">
         <v>9.369999999999999</v>
@@ -14297,10 +14289,10 @@
         <v>34039.9</v>
       </c>
       <c r="AH110" t="n">
-        <v>623.5</v>
+        <v>623.2</v>
       </c>
       <c r="AI110" t="n">
-        <v>20.7</v>
+        <v>20.2</v>
       </c>
       <c r="AJ110" t="n">
         <v>3.2</v>
@@ -14312,7 +14304,7 @@
         <v>2.1</v>
       </c>
       <c r="AM110" t="n">
-        <v>0.9</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="111">
@@ -14366,10 +14358,10 @@
         <v>1.8</v>
       </c>
       <c r="N111" t="n">
-        <v>503.5</v>
+        <v>503.2</v>
       </c>
       <c r="O111" t="n">
-        <v>49.6</v>
+        <v>49</v>
       </c>
       <c r="P111" t="n">
         <v>12.73</v>
@@ -14426,10 +14418,10 @@
         <v>17665.2</v>
       </c>
       <c r="AH111" t="n">
-        <v>526.1</v>
+        <v>525.7</v>
       </c>
       <c r="AI111" t="n">
-        <v>46.6</v>
+        <v>45.8</v>
       </c>
       <c r="AJ111" t="n">
         <v>6.5</v>
@@ -14624,10 +14616,10 @@
         <v>1.5</v>
       </c>
       <c r="N113" t="n">
-        <v>374.3</v>
+        <v>374.1</v>
       </c>
       <c r="O113" t="n">
-        <v>25.3</v>
+        <v>24.7</v>
       </c>
       <c r="P113" t="n">
         <v>37.68</v>
@@ -14657,25 +14649,25 @@
         <v>1.2</v>
       </c>
       <c r="Y113" t="n">
-        <v>369.3</v>
+        <v>369.1</v>
       </c>
       <c r="Z113" t="n">
-        <v>25.1</v>
+        <v>24.5</v>
       </c>
       <c r="AA113" t="n">
         <v>33</v>
       </c>
       <c r="AB113" t="n">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="AC113" t="n">
-        <v>2.2</v>
+        <v>0.8</v>
       </c>
       <c r="AD113" t="n">
-        <v>2.9</v>
+        <v>2.7</v>
       </c>
       <c r="AE113" t="n">
-        <v>7.1</v>
+        <v>4.1</v>
       </c>
       <c r="AF113" t="n">
         <v>18973.1</v>
@@ -14684,10 +14676,10 @@
         <v>9745.6</v>
       </c>
       <c r="AH113" t="n">
-        <v>387.7</v>
+        <v>387.4</v>
       </c>
       <c r="AI113" t="n">
-        <v>20.6</v>
+        <v>19.5</v>
       </c>
       <c r="AJ113" t="n">
         <v>3.7</v>
@@ -14753,10 +14745,10 @@
         <v>3</v>
       </c>
       <c r="N114" t="n">
-        <v>408.6</v>
+        <v>408.4</v>
       </c>
       <c r="O114" t="n">
-        <v>26.7</v>
+        <v>25.6</v>
       </c>
       <c r="P114" t="n">
         <v>13.68</v>
@@ -14786,10 +14778,10 @@
         <v>11</v>
       </c>
       <c r="Y114" t="n">
-        <v>388.7</v>
+        <v>388</v>
       </c>
       <c r="Z114" t="n">
-        <v>19.7</v>
+        <v>16</v>
       </c>
       <c r="AA114" t="n">
         <v>19.1</v>
@@ -14882,10 +14874,10 @@
         <v>4.5</v>
       </c>
       <c r="N115" t="n">
-        <v>415.6</v>
+        <v>415.2</v>
       </c>
       <c r="O115" t="n">
-        <v>29.7</v>
+        <v>27.9</v>
       </c>
       <c r="P115" t="n">
         <v>18.47</v>
@@ -14942,10 +14934,10 @@
         <v>21601.2</v>
       </c>
       <c r="AH115" t="n">
-        <v>406.6</v>
+        <v>404.9</v>
       </c>
       <c r="AI115" t="n">
-        <v>22.3</v>
+        <v>11.2</v>
       </c>
       <c r="AJ115" t="n">
         <v>6.8</v>
@@ -15049,9 +15041,7 @@
       <c r="Z116" t="n">
         <v>31.3</v>
       </c>
-      <c r="AA116" t="n">
-        <v>-53.9</v>
-      </c>
+      <c r="AA116" t="inlineStr"/>
       <c r="AB116" t="n">
         <v>3.2</v>
       </c>
@@ -15173,13 +15163,13 @@
         <v>1.7</v>
       </c>
       <c r="AC117" t="n">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
       <c r="AD117" t="n">
         <v>7.4</v>
       </c>
       <c r="AE117" t="n">
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
       <c r="AF117" t="n">
         <v>41382.4</v>
@@ -15257,10 +15247,10 @@
         <v>1.2</v>
       </c>
       <c r="N118" t="n">
-        <v>350.7</v>
+        <v>350.4</v>
       </c>
       <c r="O118" t="n">
-        <v>17.4</v>
+        <v>15.7</v>
       </c>
       <c r="P118" t="n">
         <v>37.92</v>
@@ -15290,25 +15280,25 @@
         <v>5.9</v>
       </c>
       <c r="Y118" t="n">
-        <v>350.7</v>
+        <v>350.4</v>
       </c>
       <c r="Z118" t="n">
-        <v>17.4</v>
+        <v>15.7</v>
       </c>
       <c r="AA118" t="n">
         <v>24.4</v>
       </c>
       <c r="AB118" t="n">
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="AC118" t="n">
-        <v>4.7</v>
+        <v>0.6</v>
       </c>
       <c r="AD118" t="n">
-        <v>7.9</v>
+        <v>7.5</v>
       </c>
       <c r="AE118" t="n">
-        <v>9.4</v>
+        <v>3.4</v>
       </c>
       <c r="AF118" t="n">
         <v>26896.2</v>
@@ -15374,10 +15364,10 @@
         <v>2.7</v>
       </c>
       <c r="N119" t="n">
-        <v>595.5</v>
+        <v>594.9</v>
       </c>
       <c r="O119" t="n">
-        <v>54.8</v>
+        <v>53.2</v>
       </c>
       <c r="P119" t="n">
         <v>22.53</v>
@@ -15407,25 +15397,25 @@
         <v>1.6</v>
       </c>
       <c r="Y119" t="n">
-        <v>553.1</v>
+        <v>552.3</v>
       </c>
       <c r="Z119" t="n">
-        <v>32.2</v>
+        <v>28.3</v>
       </c>
       <c r="AA119" t="n">
         <v>58.4</v>
       </c>
       <c r="AB119" t="n">
-        <v>2.5</v>
+        <v>2.2</v>
       </c>
       <c r="AC119" t="n">
-        <v>4.6</v>
+        <v>1.5</v>
       </c>
       <c r="AD119" t="n">
-        <v>4.6</v>
+        <v>4.3</v>
       </c>
       <c r="AE119" t="n">
-        <v>4.5</v>
+        <v>2.4</v>
       </c>
       <c r="AF119" t="n">
         <v>16977.4</v>
@@ -15434,10 +15424,10 @@
         <v>4065.9</v>
       </c>
       <c r="AH119" t="n">
-        <v>642.1</v>
+        <v>641.6</v>
       </c>
       <c r="AI119" t="n">
-        <v>31.7</v>
+        <v>29.9</v>
       </c>
       <c r="AJ119" t="n">
         <v>7</v>
@@ -15620,10 +15610,10 @@
         <v>5.1</v>
       </c>
       <c r="N121" t="n">
-        <v>490.8</v>
+        <v>490.5</v>
       </c>
       <c r="O121" t="n">
-        <v>64.59999999999999</v>
+        <v>64.09999999999999</v>
       </c>
       <c r="P121" t="n">
         <v>45.58</v>
@@ -15653,25 +15643,25 @@
         <v>1.9</v>
       </c>
       <c r="Y121" t="n">
-        <v>489.6</v>
+        <v>489.5</v>
       </c>
       <c r="Z121" t="n">
-        <v>66.5</v>
+        <v>66.2</v>
       </c>
       <c r="AA121" t="n">
         <v>73.90000000000001</v>
       </c>
       <c r="AB121" t="n">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="AC121" t="n">
-        <v>3.3</v>
+        <v>0.5</v>
       </c>
       <c r="AD121" t="n">
-        <v>2.4</v>
+        <v>2.2</v>
       </c>
       <c r="AE121" t="n">
-        <v>4</v>
+        <v>1.4</v>
       </c>
       <c r="AF121" t="n">
         <v>28542.8</v>
@@ -15680,22 +15670,22 @@
         <v>11887.7</v>
       </c>
       <c r="AH121" t="n">
-        <v>492.8</v>
+        <v>492.3</v>
       </c>
       <c r="AI121" t="n">
-        <v>61.1</v>
+        <v>60.3</v>
       </c>
       <c r="AJ121" t="n">
-        <v>15.9</v>
+        <v>15.6</v>
       </c>
       <c r="AK121" t="n">
-        <v>11.7</v>
+        <v>10.2</v>
       </c>
       <c r="AL121" t="n">
-        <v>6.5</v>
+        <v>6.3</v>
       </c>
       <c r="AM121" t="n">
-        <v>7.8</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="122">
@@ -15749,10 +15739,10 @@
         <v>0.4</v>
       </c>
       <c r="N122" t="n">
-        <v>358.3</v>
+        <v>357.2</v>
       </c>
       <c r="O122" t="n">
-        <v>27.5</v>
+        <v>18</v>
       </c>
       <c r="P122" t="n">
         <v>23.75</v>
@@ -15782,25 +15772,25 @@
         <v>0.8</v>
       </c>
       <c r="Y122" t="n">
-        <v>353.5</v>
+        <v>352.2</v>
       </c>
       <c r="Z122" t="n">
-        <v>26.7</v>
+        <v>13.8</v>
       </c>
       <c r="AA122" t="n">
         <v>19.2</v>
       </c>
       <c r="AB122" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="AC122" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AD122" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="AE122" t="n">
         <v>0.7</v>
-      </c>
-      <c r="AC122" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="AD122" t="n">
-        <v>3</v>
-      </c>
-      <c r="AE122" t="n">
-        <v>1.6</v>
       </c>
       <c r="AF122" t="n">
         <v>10240.8</v>
@@ -16007,10 +15997,10 @@
         <v>1.4</v>
       </c>
       <c r="N124" t="n">
-        <v>334.5</v>
+        <v>333.8</v>
       </c>
       <c r="O124" t="n">
-        <v>19.1</v>
+        <v>13.5</v>
       </c>
       <c r="P124" t="n">
         <v>8.880000000000001</v>
@@ -16040,25 +16030,25 @@
         <v>1.9</v>
       </c>
       <c r="Y124" t="n">
-        <v>333.2</v>
+        <v>332.2</v>
       </c>
       <c r="Z124" t="n">
-        <v>22.1</v>
+        <v>15.4</v>
       </c>
       <c r="AA124" t="n">
         <v>18.6</v>
       </c>
       <c r="AB124" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="AC124" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AD124" t="n">
+        <v>8.6</v>
+      </c>
+      <c r="AE124" t="n">
         <v>1.8</v>
-      </c>
-      <c r="AC124" t="n">
-        <v>3</v>
-      </c>
-      <c r="AD124" t="n">
-        <v>8.9</v>
-      </c>
-      <c r="AE124" t="n">
-        <v>5.3</v>
       </c>
       <c r="AF124" t="n">
         <v>24146.7</v>
@@ -16136,10 +16126,10 @@
         <v>4.9</v>
       </c>
       <c r="N125" t="n">
-        <v>354.6</v>
+        <v>354.4</v>
       </c>
       <c r="O125" t="n">
-        <v>31.3</v>
+        <v>30.5</v>
       </c>
       <c r="P125" t="n">
         <v>49.18</v>
@@ -16169,25 +16159,25 @@
         <v>9.800000000000001</v>
       </c>
       <c r="Y125" t="n">
-        <v>348.7</v>
+        <v>348.6</v>
       </c>
       <c r="Z125" t="n">
-        <v>27</v>
+        <v>26.6</v>
       </c>
       <c r="AA125" t="n">
         <v>34.7</v>
       </c>
       <c r="AB125" t="n">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="AC125" t="n">
-        <v>1.5</v>
+        <v>1.2</v>
       </c>
       <c r="AD125" t="n">
         <v>6.6</v>
       </c>
       <c r="AE125" t="n">
-        <v>4.6</v>
+        <v>4.2</v>
       </c>
       <c r="AF125" t="n">
         <v>31322</v>
@@ -16196,10 +16186,10 @@
         <v>19600.1</v>
       </c>
       <c r="AH125" t="n">
-        <v>377.7</v>
+        <v>377</v>
       </c>
       <c r="AI125" t="n">
-        <v>35.9</v>
+        <v>33.8</v>
       </c>
       <c r="AJ125" t="n">
         <v>17.6</v>
@@ -16208,10 +16198,10 @@
         <v>3.7</v>
       </c>
       <c r="AL125" t="n">
-        <v>4.2</v>
+        <v>4.1</v>
       </c>
       <c r="AM125" t="n">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="126">
@@ -16265,10 +16255,10 @@
         <v>4.1</v>
       </c>
       <c r="N126" t="n">
-        <v>293.8</v>
+        <v>293.4</v>
       </c>
       <c r="O126" t="n">
-        <v>18.2</v>
+        <v>16.1</v>
       </c>
       <c r="P126" t="n">
         <v>18.7</v>
@@ -16298,25 +16288,25 @@
         <v>6.1</v>
       </c>
       <c r="Y126" t="n">
-        <v>308.4</v>
+        <v>307.7</v>
       </c>
       <c r="Z126" t="n">
-        <v>17.4</v>
+        <v>12.4</v>
       </c>
       <c r="AA126" t="n">
         <v>-14.9</v>
       </c>
       <c r="AB126" t="n">
-        <v>2.4</v>
+        <v>2.2</v>
       </c>
       <c r="AC126" t="n">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="AD126" t="n">
-        <v>14.6</v>
+        <v>13.9</v>
       </c>
       <c r="AE126" t="n">
-        <v>8.6</v>
+        <v>3.5</v>
       </c>
       <c r="AF126" t="n">
         <v>68214.3</v>
@@ -16394,7 +16384,7 @@
         <v>9</v>
       </c>
       <c r="N127" t="n">
-        <v>600.8</v>
+        <v>600.7</v>
       </c>
       <c r="O127" t="n">
         <v>81</v>
@@ -16427,10 +16417,10 @@
         <v>6.1</v>
       </c>
       <c r="Y127" t="n">
-        <v>594.8</v>
+        <v>594.6</v>
       </c>
       <c r="Z127" t="n">
-        <v>85.8</v>
+        <v>85.7</v>
       </c>
       <c r="AA127" t="n">
         <v>81.40000000000001</v>
@@ -16445,7 +16435,7 @@
         <v>3.6</v>
       </c>
       <c r="AE127" t="n">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="AF127" t="n">
         <v>57425</v>
@@ -16454,10 +16444,10 @@
         <v>73141.8</v>
       </c>
       <c r="AH127" t="n">
-        <v>637</v>
+        <v>637.4</v>
       </c>
       <c r="AI127" t="n">
-        <v>16.1</v>
+        <v>14.7</v>
       </c>
       <c r="AJ127" t="n">
         <v>18.9</v>
@@ -16466,10 +16456,10 @@
         <v>3.4</v>
       </c>
       <c r="AL127" t="n">
-        <v>12.8</v>
+        <v>12.9</v>
       </c>
       <c r="AM127" t="n">
-        <v>2.2</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="128">
@@ -16523,10 +16513,10 @@
         <v>2.9</v>
       </c>
       <c r="N128" t="n">
-        <v>450.7</v>
+        <v>447.5</v>
       </c>
       <c r="O128" t="n">
-        <v>34</v>
+        <v>19.7</v>
       </c>
       <c r="P128" t="n">
         <v>14.65</v>
@@ -16556,31 +16546,31 @@
         <v>6.4</v>
       </c>
       <c r="Y128" t="n">
-        <v>449.3</v>
+        <v>445.8</v>
       </c>
       <c r="Z128" t="n">
-        <v>34.5</v>
+        <v>19.1</v>
       </c>
       <c r="AA128" t="n">
         <v>10.9</v>
       </c>
       <c r="AB128" t="n">
-        <v>5.7</v>
+        <v>5.1</v>
       </c>
       <c r="AC128" t="n">
-        <v>5.8</v>
+        <v>2.9</v>
       </c>
       <c r="AD128" t="n">
-        <v>15.6</v>
+        <v>15.2</v>
       </c>
       <c r="AE128" t="n">
-        <v>8.9</v>
+        <v>7.6</v>
       </c>
       <c r="AF128" t="n">
-        <v>34689</v>
+        <v>32785</v>
       </c>
       <c r="AG128" t="n">
-        <v>33570.5</v>
+        <v>19594.8</v>
       </c>
       <c r="AH128" t="n">
         <v>473</v>
@@ -16652,10 +16642,10 @@
         <v>2.5</v>
       </c>
       <c r="N129" t="n">
-        <v>395.9</v>
+        <v>395.2</v>
       </c>
       <c r="O129" t="n">
-        <v>28.6</v>
+        <v>24.3</v>
       </c>
       <c r="P129" t="n">
         <v>26.65</v>
@@ -16685,23 +16675,23 @@
         <v>2.9</v>
       </c>
       <c r="Y129" t="n">
-        <v>392.8</v>
+        <v>391.9</v>
       </c>
       <c r="Z129" t="n">
-        <v>31.7</v>
+        <v>26.4</v>
       </c>
       <c r="AA129" t="inlineStr"/>
       <c r="AB129" t="n">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="AC129" t="n">
-        <v>2.5</v>
+        <v>1.6</v>
       </c>
       <c r="AD129" t="n">
-        <v>13.6</v>
+        <v>13.5</v>
       </c>
       <c r="AE129" t="n">
-        <v>6.2</v>
+        <v>5.5</v>
       </c>
       <c r="AF129" t="n">
         <v>21774.6</v>
@@ -16779,10 +16769,10 @@
         <v>2.1</v>
       </c>
       <c r="N130" t="n">
-        <v>399.6</v>
+        <v>397.4</v>
       </c>
       <c r="O130" t="n">
-        <v>27.3</v>
+        <v>12.8</v>
       </c>
       <c r="P130" t="n">
         <v>15.88</v>
@@ -16812,25 +16802,25 @@
         <v>1.3</v>
       </c>
       <c r="Y130" t="n">
-        <v>403.3</v>
+        <v>400.8</v>
       </c>
       <c r="Z130" t="n">
-        <v>28.7</v>
+        <v>10.3</v>
       </c>
       <c r="AA130" t="n">
         <v>-3.9</v>
       </c>
       <c r="AB130" t="n">
-        <v>3.1</v>
+        <v>2.5</v>
       </c>
       <c r="AC130" t="n">
-        <v>7.3</v>
+        <v>0.6</v>
       </c>
       <c r="AD130" t="n">
-        <v>9.9</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="AE130" t="n">
-        <v>7.7</v>
+        <v>2.1</v>
       </c>
       <c r="AF130" t="n">
         <v>34325</v>
@@ -16839,10 +16829,10 @@
         <v>12717.9</v>
       </c>
       <c r="AH130" t="n">
-        <v>393.4</v>
+        <v>391.9</v>
       </c>
       <c r="AI130" t="n">
-        <v>23.7</v>
+        <v>14.5</v>
       </c>
       <c r="AJ130" t="n">
         <v>18.3</v>
@@ -16854,7 +16844,7 @@
         <v>4.7</v>
       </c>
       <c r="AM130" t="n">
-        <v>1.2</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="131">
@@ -16908,10 +16898,10 @@
         <v>3.8</v>
       </c>
       <c r="N131" t="n">
-        <v>387.6</v>
+        <v>387.1</v>
       </c>
       <c r="O131" t="n">
-        <v>26.1</v>
+        <v>24.3</v>
       </c>
       <c r="P131" t="n">
         <v>34.57</v>
@@ -16941,10 +16931,10 @@
         <v>10.9</v>
       </c>
       <c r="Y131" t="n">
-        <v>391.3</v>
+        <v>391.1</v>
       </c>
       <c r="Z131" t="n">
-        <v>28</v>
+        <v>26.9</v>
       </c>
       <c r="AA131" t="n">
         <v>9.199999999999999</v>
@@ -16953,13 +16943,13 @@
         <v>4.2</v>
       </c>
       <c r="AC131" t="n">
-        <v>2.8</v>
+        <v>2.4</v>
       </c>
       <c r="AD131" t="n">
-        <v>15.9</v>
+        <v>15.8</v>
       </c>
       <c r="AE131" t="n">
-        <v>8</v>
+        <v>7.9</v>
       </c>
       <c r="AF131" t="n">
         <v>32759.3</v>
@@ -16968,22 +16958,22 @@
         <v>16241.3</v>
       </c>
       <c r="AH131" t="n">
-        <v>378.3</v>
+        <v>377.1</v>
       </c>
       <c r="AI131" t="n">
-        <v>17.5</v>
+        <v>10.5</v>
       </c>
       <c r="AJ131" t="n">
-        <v>19.5</v>
+        <v>17.2</v>
       </c>
       <c r="AK131" t="n">
-        <v>18.8</v>
+        <v>5.9</v>
       </c>
       <c r="AL131" t="n">
-        <v>5</v>
+        <v>4.1</v>
       </c>
       <c r="AM131" t="n">
-        <v>9.1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="132">
@@ -17166,10 +17156,10 @@
         <v>0.9</v>
       </c>
       <c r="N133" t="n">
-        <v>383.5</v>
+        <v>383.4</v>
       </c>
       <c r="O133" t="n">
-        <v>13.1</v>
+        <v>11.6</v>
       </c>
       <c r="P133" t="n">
         <v>27.38</v>
@@ -17199,23 +17189,23 @@
         <v>0.9</v>
       </c>
       <c r="Y133" t="n">
-        <v>382.2</v>
+        <v>382.1</v>
       </c>
       <c r="Z133" t="n">
-        <v>13.1</v>
+        <v>11.4</v>
       </c>
       <c r="AA133" t="inlineStr"/>
       <c r="AB133" t="n">
         <v>1.7</v>
       </c>
       <c r="AC133" t="n">
-        <v>1.5</v>
+        <v>0.4</v>
       </c>
       <c r="AD133" t="n">
-        <v>7</v>
+        <v>6.9</v>
       </c>
       <c r="AE133" t="n">
-        <v>2.3</v>
+        <v>1.2</v>
       </c>
       <c r="AF133" t="n">
         <v>15606.3</v>
@@ -17420,10 +17410,10 @@
         <v>8.800000000000001</v>
       </c>
       <c r="N135" t="n">
-        <v>612.8</v>
+        <v>612.5</v>
       </c>
       <c r="O135" t="n">
-        <v>56.8</v>
+        <v>56.7</v>
       </c>
       <c r="P135" t="n">
         <v>34.67</v>
@@ -17453,10 +17443,10 @@
         <v>4.4</v>
       </c>
       <c r="Y135" t="n">
-        <v>598.6</v>
+        <v>598.3</v>
       </c>
       <c r="Z135" t="n">
-        <v>51.9</v>
+        <v>51.8</v>
       </c>
       <c r="AA135" t="n">
         <v>61.5</v>
@@ -17465,37 +17455,37 @@
         <v>1.3</v>
       </c>
       <c r="AC135" t="n">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="AD135" t="n">
-        <v>2.2</v>
+        <v>2.1</v>
       </c>
       <c r="AE135" t="n">
-        <v>2.6</v>
+        <v>1.4</v>
       </c>
       <c r="AF135" t="n">
-        <v>167940.7</v>
+        <v>150311.2</v>
       </c>
       <c r="AG135" t="n">
-        <v>211865</v>
+        <v>168974.6</v>
       </c>
       <c r="AH135" t="n">
-        <v>669.9</v>
+        <v>670.1</v>
       </c>
       <c r="AI135" t="n">
-        <v>35.5</v>
+        <v>35.1</v>
       </c>
       <c r="AJ135" t="n">
-        <v>31.6</v>
+        <v>31.5</v>
       </c>
       <c r="AK135" t="n">
         <v>15.4</v>
       </c>
       <c r="AL135" t="n">
-        <v>23.1</v>
+        <v>23</v>
       </c>
       <c r="AM135" t="n">
-        <v>11</v>
+        <v>10.9</v>
       </c>
     </row>
     <row r="136">
@@ -17549,10 +17539,10 @@
         <v>4.4</v>
       </c>
       <c r="N136" t="n">
-        <v>493.3</v>
+        <v>492.2</v>
       </c>
       <c r="O136" t="n">
-        <v>67.2</v>
+        <v>65.2</v>
       </c>
       <c r="P136" t="n">
         <v>39.35</v>
@@ -17582,25 +17572,25 @@
         <v>8.5</v>
       </c>
       <c r="Y136" t="n">
-        <v>468.2</v>
+        <v>468.1</v>
       </c>
       <c r="Z136" t="n">
-        <v>50.9</v>
+        <v>50.8</v>
       </c>
       <c r="AA136" t="n">
         <v>70.7</v>
       </c>
       <c r="AB136" t="n">
-        <v>4.9</v>
+        <v>4.8</v>
       </c>
       <c r="AC136" t="n">
-        <v>3.2</v>
+        <v>2</v>
       </c>
       <c r="AD136" t="n">
-        <v>13</v>
+        <v>12.8</v>
       </c>
       <c r="AE136" t="n">
-        <v>5.6</v>
+        <v>4</v>
       </c>
       <c r="AF136" t="n">
         <v>19340.6</v>
@@ -17609,10 +17599,10 @@
         <v>8851.6</v>
       </c>
       <c r="AH136" t="n">
-        <v>583.6</v>
+        <v>581.1</v>
       </c>
       <c r="AI136" t="n">
-        <v>31.5</v>
+        <v>17.7</v>
       </c>
       <c r="AJ136" t="n">
         <v>6.2</v>
@@ -17621,10 +17611,10 @@
         <v>1.7</v>
       </c>
       <c r="AL136" t="n">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="AM136" t="n">
-        <v>1.2</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="137">
@@ -17723,13 +17713,13 @@
         <v>4.9</v>
       </c>
       <c r="AC137" t="n">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="AD137" t="n">
-        <v>16.7</v>
+        <v>16.5</v>
       </c>
       <c r="AE137" t="n">
-        <v>6.1</v>
+        <v>5.7</v>
       </c>
       <c r="AF137" t="n">
         <v>65499.5</v>
@@ -17795,10 +17785,10 @@
         <v>1.8</v>
       </c>
       <c r="N138" t="n">
-        <v>407.5</v>
+        <v>407.4</v>
       </c>
       <c r="O138" t="n">
-        <v>54</v>
+        <v>53.8</v>
       </c>
       <c r="P138" t="n">
         <v>72</v>
@@ -17828,25 +17818,25 @@
         <v>2.5</v>
       </c>
       <c r="Y138" t="n">
-        <v>391.9</v>
+        <v>391.7</v>
       </c>
       <c r="Z138" t="n">
-        <v>49</v>
+        <v>48.6</v>
       </c>
       <c r="AA138" t="n">
         <v>62.7</v>
       </c>
       <c r="AB138" t="n">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="AC138" t="n">
-        <v>3.1</v>
+        <v>0.6</v>
       </c>
       <c r="AD138" t="n">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="AE138" t="n">
-        <v>4.2</v>
+        <v>1.6</v>
       </c>
       <c r="AF138" t="n">
         <v>31662.6</v>
@@ -17861,16 +17851,16 @@
         <v>20.1</v>
       </c>
       <c r="AJ138" t="n">
-        <v>14.5</v>
+        <v>13.9</v>
       </c>
       <c r="AK138" t="n">
-        <v>8.199999999999999</v>
+        <v>3.3</v>
       </c>
       <c r="AL138" t="n">
-        <v>5.4</v>
+        <v>5.2</v>
       </c>
       <c r="AM138" t="n">
-        <v>3.3</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="139">
@@ -17927,7 +17917,7 @@
         <v>562.8</v>
       </c>
       <c r="O139" t="n">
-        <v>57</v>
+        <v>57.1</v>
       </c>
       <c r="P139" t="n">
         <v>33.6</v>
@@ -17978,16 +17968,16 @@
         <v>0.7</v>
       </c>
       <c r="AF139" t="n">
-        <v>47973.5</v>
+        <v>46013.1</v>
       </c>
       <c r="AG139" t="n">
-        <v>53109.2</v>
+        <v>44566.7</v>
       </c>
       <c r="AH139" t="n">
-        <v>611.4</v>
+        <v>611.8</v>
       </c>
       <c r="AI139" t="n">
-        <v>48.3</v>
+        <v>48.2</v>
       </c>
       <c r="AJ139" t="n">
         <v>6.7</v>
@@ -18098,13 +18088,13 @@
         <v>2.4</v>
       </c>
       <c r="AC140" t="n">
-        <v>2.2</v>
+        <v>1.8</v>
       </c>
       <c r="AD140" t="n">
-        <v>8.9</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="AE140" t="n">
-        <v>8.699999999999999</v>
+        <v>6.5</v>
       </c>
       <c r="AF140" t="n">
         <v>47977.7</v>
@@ -18113,22 +18103,22 @@
         <v>33463</v>
       </c>
       <c r="AH140" t="n">
-        <v>445.3</v>
+        <v>445.4</v>
       </c>
       <c r="AI140" t="n">
-        <v>37.2</v>
+        <v>37.1</v>
       </c>
       <c r="AJ140" t="n">
-        <v>38.6</v>
+        <v>37.7</v>
       </c>
       <c r="AK140" t="n">
-        <v>15.8</v>
+        <v>13.7</v>
       </c>
       <c r="AL140" t="n">
-        <v>12.6</v>
+        <v>12.4</v>
       </c>
       <c r="AM140" t="n">
-        <v>4.5</v>
+        <v>4.1</v>
       </c>
     </row>
     <row r="141">
@@ -18182,10 +18172,10 @@
         <v>2.3</v>
       </c>
       <c r="N141" t="n">
-        <v>446.9</v>
+        <v>446.1</v>
       </c>
       <c r="O141" t="n">
-        <v>27.4</v>
+        <v>23.6</v>
       </c>
       <c r="P141" t="n">
         <v>17.17</v>
@@ -18242,22 +18232,22 @@
         <v>66030.8</v>
       </c>
       <c r="AH141" t="n">
-        <v>448.5</v>
+        <v>447</v>
       </c>
       <c r="AI141" t="n">
-        <v>34.9</v>
+        <v>29</v>
       </c>
       <c r="AJ141" t="n">
-        <v>18.2</v>
+        <v>17.9</v>
       </c>
       <c r="AK141" t="n">
-        <v>7.1</v>
+        <v>5.1</v>
       </c>
       <c r="AL141" t="n">
-        <v>6.2</v>
+        <v>6.1</v>
       </c>
       <c r="AM141" t="n">
-        <v>3.7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="142">
@@ -18311,10 +18301,10 @@
         <v>2.6</v>
       </c>
       <c r="N142" t="n">
-        <v>358.4</v>
+        <v>358.1</v>
       </c>
       <c r="O142" t="n">
-        <v>16.6</v>
+        <v>15.3</v>
       </c>
       <c r="P142" t="n">
         <v>33.03</v>
@@ -18344,25 +18334,25 @@
         <v>5.8</v>
       </c>
       <c r="Y142" t="n">
-        <v>359.3</v>
+        <v>359</v>
       </c>
       <c r="Z142" t="n">
-        <v>15.6</v>
+        <v>13.6</v>
       </c>
       <c r="AA142" t="n">
         <v>23.4</v>
       </c>
       <c r="AB142" t="n">
-        <v>3.7</v>
+        <v>3.5</v>
       </c>
       <c r="AC142" t="n">
-        <v>4.1</v>
+        <v>0.9</v>
       </c>
       <c r="AD142" t="n">
-        <v>16.7</v>
+        <v>16.3</v>
       </c>
       <c r="AE142" t="n">
-        <v>10.1</v>
+        <v>4.6</v>
       </c>
       <c r="AF142" t="n">
         <v>50529.5</v>
@@ -18440,10 +18430,10 @@
         <v>1.5</v>
       </c>
       <c r="N143" t="n">
-        <v>414.2</v>
+        <v>413.2</v>
       </c>
       <c r="O143" t="n">
-        <v>46.1</v>
+        <v>42.5</v>
       </c>
       <c r="P143" t="n">
         <v>25.03</v>
@@ -18485,13 +18475,13 @@
         <v>1.9</v>
       </c>
       <c r="AC143" t="n">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="AD143" t="n">
-        <v>7</v>
+        <v>6.8</v>
       </c>
       <c r="AE143" t="n">
-        <v>3.4</v>
+        <v>1.5</v>
       </c>
       <c r="AF143" t="n">
         <v>26530.4</v>
@@ -18500,10 +18490,10 @@
         <v>11155.7</v>
       </c>
       <c r="AH143" t="n">
-        <v>486.1</v>
+        <v>479.1</v>
       </c>
       <c r="AI143" t="n">
-        <v>50.5</v>
+        <v>7.3</v>
       </c>
       <c r="AJ143" t="n">
         <v>6.8</v>
@@ -18512,10 +18502,10 @@
         <v>2</v>
       </c>
       <c r="AL143" t="n">
-        <v>2.9</v>
+        <v>2.5</v>
       </c>
       <c r="AM143" t="n">
-        <v>3.3</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="144">
@@ -18698,10 +18688,10 @@
         <v>3</v>
       </c>
       <c r="N145" t="n">
-        <v>405.9</v>
+        <v>405.4</v>
       </c>
       <c r="O145" t="n">
-        <v>22.3</v>
+        <v>17.2</v>
       </c>
       <c r="P145" t="n">
         <v>28.22</v>
@@ -18731,23 +18721,23 @@
         <v>4.4</v>
       </c>
       <c r="Y145" t="n">
-        <v>405</v>
+        <v>405.1</v>
       </c>
       <c r="Z145" t="n">
-        <v>17.3</v>
+        <v>17.2</v>
       </c>
       <c r="AA145" t="inlineStr"/>
       <c r="AB145" t="n">
-        <v>4.1</v>
+        <v>4</v>
       </c>
       <c r="AC145" t="n">
-        <v>2.4</v>
+        <v>2.3</v>
       </c>
       <c r="AD145" t="n">
-        <v>15</v>
+        <v>14.8</v>
       </c>
       <c r="AE145" t="n">
-        <v>9</v>
+        <v>8.5</v>
       </c>
       <c r="AF145" t="n">
         <v>19460.4</v>
@@ -18756,10 +18746,10 @@
         <v>6210.8</v>
       </c>
       <c r="AH145" t="n">
-        <v>446.3</v>
+        <v>422.3</v>
       </c>
       <c r="AI145" t="n">
-        <v>91.2</v>
+        <v>3.8</v>
       </c>
       <c r="AJ145" t="n">
         <v>10.6</v>
@@ -18768,10 +18758,10 @@
         <v>1.4</v>
       </c>
       <c r="AL145" t="n">
-        <v>3.7</v>
+        <v>3</v>
       </c>
       <c r="AM145" t="n">
-        <v>2.4</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="146">
@@ -18825,10 +18815,10 @@
         <v>6</v>
       </c>
       <c r="N146" t="n">
-        <v>522.5</v>
+        <v>522.4</v>
       </c>
       <c r="O146" t="n">
-        <v>49.9</v>
+        <v>48.6</v>
       </c>
       <c r="P146" t="n">
         <v>10.15</v>
@@ -18858,10 +18848,10 @@
         <v>7.7</v>
       </c>
       <c r="Y146" t="n">
-        <v>542.9</v>
+        <v>542.4</v>
       </c>
       <c r="Z146" t="n">
-        <v>34</v>
+        <v>32.9</v>
       </c>
       <c r="AA146" t="n">
         <v>-48</v>
@@ -18885,22 +18875,22 @@
         <v>210819.7</v>
       </c>
       <c r="AH146" t="n">
-        <v>446.7</v>
+        <v>447.6</v>
       </c>
       <c r="AI146" t="n">
-        <v>10.9</v>
+        <v>7.6</v>
       </c>
       <c r="AJ146" t="n">
-        <v>45.6</v>
+        <v>43.1</v>
       </c>
       <c r="AK146" t="n">
-        <v>25.8</v>
+        <v>22.7</v>
       </c>
       <c r="AL146" t="n">
-        <v>15.1</v>
+        <v>14.4</v>
       </c>
       <c r="AM146" t="n">
-        <v>8.300000000000001</v>
+        <v>7.2</v>
       </c>
     </row>
     <row r="147">
@@ -19149,16 +19139,16 @@
         <v>30.8</v>
       </c>
       <c r="AJ148" t="n">
-        <v>23.8</v>
+        <v>23.6</v>
       </c>
       <c r="AK148" t="n">
-        <v>13.6</v>
+        <v>13.4</v>
       </c>
       <c r="AL148" t="n">
-        <v>6.4</v>
+        <v>6.3</v>
       </c>
       <c r="AM148" t="n">
-        <v>2.9</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="149">
@@ -19212,10 +19202,10 @@
         <v>1.5</v>
       </c>
       <c r="N149" t="n">
-        <v>308.2</v>
+        <v>308</v>
       </c>
       <c r="O149" t="n">
-        <v>12.7</v>
+        <v>11</v>
       </c>
       <c r="P149" t="n">
         <v>22.03</v>
@@ -19245,10 +19235,10 @@
         <v>1.9</v>
       </c>
       <c r="Y149" t="n">
-        <v>305.4</v>
+        <v>305.2</v>
       </c>
       <c r="Z149" t="n">
-        <v>11</v>
+        <v>9.6</v>
       </c>
       <c r="AA149" t="n">
         <v>14.1</v>
@@ -19257,13 +19247,13 @@
         <v>1.8</v>
       </c>
       <c r="AC149" t="n">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="AD149" t="n">
-        <v>11.9</v>
+        <v>11.6</v>
       </c>
       <c r="AE149" t="n">
-        <v>4.5</v>
+        <v>3.3</v>
       </c>
       <c r="AF149" t="n">
         <v>28381.6</v>
@@ -19272,22 +19262,22 @@
         <v>7563.6</v>
       </c>
       <c r="AH149" t="n">
-        <v>312.2</v>
+        <v>312</v>
       </c>
       <c r="AI149" t="n">
-        <v>13.7</v>
+        <v>11.7</v>
       </c>
       <c r="AJ149" t="n">
-        <v>16</v>
+        <v>15.6</v>
       </c>
       <c r="AK149" t="n">
-        <v>7.9</v>
+        <v>4.1</v>
       </c>
       <c r="AL149" t="n">
-        <v>2.7</v>
+        <v>2.5</v>
       </c>
       <c r="AM149" t="n">
-        <v>2.6</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="150">
@@ -19341,10 +19331,10 @@
         <v>6.2</v>
       </c>
       <c r="N150" t="n">
-        <v>395.3</v>
+        <v>394.7</v>
       </c>
       <c r="O150" t="n">
-        <v>30.5</v>
+        <v>28.2</v>
       </c>
       <c r="P150" t="n">
         <v>32.4</v>
@@ -19374,10 +19364,10 @@
         <v>8.1</v>
       </c>
       <c r="Y150" t="n">
-        <v>386.9</v>
+        <v>386.7</v>
       </c>
       <c r="Z150" t="n">
-        <v>25.2</v>
+        <v>24.9</v>
       </c>
       <c r="AA150" t="n">
         <v>37.7</v>
@@ -19401,22 +19391,22 @@
         <v>21422.1</v>
       </c>
       <c r="AH150" t="n">
-        <v>429.8</v>
+        <v>428.1</v>
       </c>
       <c r="AI150" t="n">
-        <v>25.9</v>
+        <v>11.8</v>
       </c>
       <c r="AJ150" t="n">
-        <v>24.3</v>
+        <v>23.8</v>
       </c>
       <c r="AK150" t="n">
-        <v>10.1</v>
+        <v>6.5</v>
       </c>
       <c r="AL150" t="n">
-        <v>7.7</v>
+        <v>7.4</v>
       </c>
       <c r="AM150" t="n">
-        <v>4.7</v>
+        <v>2.3</v>
       </c>
     </row>
     <row r="151">
@@ -19536,16 +19526,16 @@
         <v>5</v>
       </c>
       <c r="AJ151" t="n">
-        <v>16.1</v>
+        <v>15.3</v>
       </c>
       <c r="AK151" t="n">
-        <v>7.8</v>
+        <v>5.4</v>
       </c>
       <c r="AL151" t="n">
-        <v>4.8</v>
+        <v>4.5</v>
       </c>
       <c r="AM151" t="n">
-        <v>2.3</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="152">
@@ -19728,10 +19718,10 @@
         <v>1</v>
       </c>
       <c r="N153" t="n">
-        <v>405.3</v>
+        <v>405.9</v>
       </c>
       <c r="O153" t="n">
-        <v>25.4</v>
+        <v>22.9</v>
       </c>
       <c r="P153" t="n">
         <v>19.67</v>
@@ -19761,10 +19751,10 @@
         <v>2.6</v>
       </c>
       <c r="Y153" t="n">
-        <v>401.3</v>
+        <v>401.9</v>
       </c>
       <c r="Z153" t="n">
-        <v>23.2</v>
+        <v>20.2</v>
       </c>
       <c r="AA153" t="n">
         <v>31.4</v>
@@ -19899,7 +19889,7 @@
         <v>-9</v>
       </c>
       <c r="AB154" t="n">
-        <v>2.7</v>
+        <v>2.6</v>
       </c>
       <c r="AC154" t="n">
         <v>1.7</v>
@@ -19908,7 +19898,7 @@
         <v>12.1</v>
       </c>
       <c r="AE154" t="n">
-        <v>6.9</v>
+        <v>6.8</v>
       </c>
       <c r="AF154" t="n">
         <v>56576.9</v>
@@ -19923,16 +19913,16 @@
         <v>8.800000000000001</v>
       </c>
       <c r="AJ154" t="n">
-        <v>49.5</v>
+        <v>48.2</v>
       </c>
       <c r="AK154" t="n">
-        <v>19.9</v>
+        <v>15.9</v>
       </c>
       <c r="AL154" t="n">
-        <v>11.6</v>
+        <v>11.3</v>
       </c>
       <c r="AM154" t="n">
-        <v>5.2</v>
+        <v>4.1</v>
       </c>
     </row>
     <row r="155">
@@ -19986,10 +19976,10 @@
         <v>4.3</v>
       </c>
       <c r="N155" t="n">
-        <v>517.8</v>
+        <v>516.8</v>
       </c>
       <c r="O155" t="n">
-        <v>69.5</v>
+        <v>64.59999999999999</v>
       </c>
       <c r="P155" t="n">
         <v>28.78</v>
@@ -20019,10 +20009,10 @@
         <v>7.9</v>
       </c>
       <c r="Y155" t="n">
-        <v>538</v>
+        <v>536.7</v>
       </c>
       <c r="Z155" t="n">
-        <v>54</v>
+        <v>47.4</v>
       </c>
       <c r="AA155" t="n">
         <v>9.699999999999999</v>
@@ -20040,28 +20030,28 @@
         <v>2.2</v>
       </c>
       <c r="AF155" t="n">
-        <v>86755.89999999999</v>
+        <v>85409.89999999999</v>
       </c>
       <c r="AG155" t="n">
-        <v>112169.5</v>
+        <v>108672.3</v>
       </c>
       <c r="AH155" t="n">
-        <v>410.4</v>
+        <v>408.3</v>
       </c>
       <c r="AI155" t="n">
-        <v>36.6</v>
+        <v>26.2</v>
       </c>
       <c r="AJ155" t="n">
-        <v>30.7</v>
+        <v>29.5</v>
       </c>
       <c r="AK155" t="n">
-        <v>13.6</v>
+        <v>12.5</v>
       </c>
       <c r="AL155" t="n">
-        <v>8.699999999999999</v>
+        <v>8</v>
       </c>
       <c r="AM155" t="n">
-        <v>4.6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="156">
@@ -20115,10 +20105,10 @@
         <v>2.4</v>
       </c>
       <c r="N156" t="n">
-        <v>541.2</v>
+        <v>538.1</v>
       </c>
       <c r="O156" t="n">
-        <v>55.7</v>
+        <v>36.9</v>
       </c>
       <c r="P156" t="n">
         <v>4.38</v>
@@ -20148,17 +20138,17 @@
         <v>3.4</v>
       </c>
       <c r="Y156" t="n">
-        <v>510.2</v>
+        <v>505.6</v>
       </c>
       <c r="Z156" t="n">
-        <v>40</v>
+        <v>16.5</v>
       </c>
       <c r="AA156" t="inlineStr"/>
       <c r="AB156" t="n">
         <v>2.6</v>
       </c>
       <c r="AC156" t="n">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="AD156" t="n">
         <v>6</v>
@@ -20167,16 +20157,16 @@
         <v>1</v>
       </c>
       <c r="AF156" t="n">
-        <v>926291.3</v>
+        <v>927371.4</v>
       </c>
       <c r="AG156" t="n">
-        <v>172281.7</v>
+        <v>167504</v>
       </c>
       <c r="AH156" t="n">
-        <v>566.3</v>
+        <v>562.2</v>
       </c>
       <c r="AI156" t="n">
-        <v>54</v>
+        <v>28.3</v>
       </c>
       <c r="AJ156" t="n">
         <v>12.3</v>
@@ -20185,10 +20175,10 @@
         <v>2.3</v>
       </c>
       <c r="AL156" t="n">
-        <v>6.8</v>
+        <v>6.6</v>
       </c>
       <c r="AM156" t="n">
-        <v>3.1</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="157">
@@ -20242,10 +20232,10 @@
         <v>5.9</v>
       </c>
       <c r="N157" t="n">
-        <v>758.8</v>
+        <v>759</v>
       </c>
       <c r="O157" t="n">
-        <v>49.7</v>
+        <v>49.5</v>
       </c>
       <c r="P157" t="n">
         <v>3.2</v>
@@ -20302,10 +20292,10 @@
         <v>38160.4</v>
       </c>
       <c r="AH157" t="n">
-        <v>758.5</v>
+        <v>758.8</v>
       </c>
       <c r="AI157" t="n">
-        <v>55.1</v>
+        <v>55</v>
       </c>
       <c r="AJ157" t="n">
         <v>3.7</v>
@@ -20314,7 +20304,7 @@
         <v>1.6</v>
       </c>
       <c r="AL157" t="n">
-        <v>3.6</v>
+        <v>3.7</v>
       </c>
       <c r="AM157" t="n">
         <v>1.6</v>

</xml_diff>

<commit_message>
fixed HELCATS data file
</commit_message>
<xml_diff>
--- a/icmecat/HELCATS_ICMECAT_v20.xlsx
+++ b/icmecat/HELCATS_ICMECAT_v20.xlsx
@@ -57040,10 +57040,10 @@
         <v>1.4</v>
       </c>
       <c r="N457" t="n">
-        <v>423.7</v>
+        <v>414.5</v>
       </c>
       <c r="O457" t="n">
-        <v>7</v>
+        <v>10.3</v>
       </c>
       <c r="P457" t="n">
         <v>8.07</v>
@@ -57073,29 +57073,31 @@
         <v>1.2</v>
       </c>
       <c r="Y457" t="n">
-        <v>423.7</v>
+        <v>414.5</v>
       </c>
       <c r="Z457" t="n">
-        <v>7</v>
-      </c>
-      <c r="AA457" t="inlineStr"/>
+        <v>10.3</v>
+      </c>
+      <c r="AA457" t="n">
+        <v>11.9</v>
+      </c>
       <c r="AB457" t="n">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="AC457" t="n">
         <v>0.5</v>
       </c>
       <c r="AD457" t="n">
-        <v>6.4</v>
+        <v>6.9</v>
       </c>
       <c r="AE457" t="n">
-        <v>1.6</v>
+        <v>1.7</v>
       </c>
       <c r="AF457" t="n">
-        <v>26525.1</v>
+        <v>29813.9</v>
       </c>
       <c r="AG457" t="n">
-        <v>7917.9</v>
+        <v>6647.6</v>
       </c>
       <c r="AH457" t="inlineStr"/>
       <c r="AI457" t="inlineStr"/>
@@ -57155,10 +57157,10 @@
         <v>1.1</v>
       </c>
       <c r="N458" t="n">
-        <v>-0</v>
+        <v>370.7</v>
       </c>
       <c r="O458" t="n">
-        <v>0</v>
+        <v>20.1</v>
       </c>
       <c r="P458" t="n">
         <v>13.25</v>
@@ -57188,26 +57190,32 @@
         <v>2.4</v>
       </c>
       <c r="Y458" t="n">
-        <v>-0</v>
+        <v>370.7</v>
       </c>
       <c r="Z458" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA458" t="inlineStr"/>
+        <v>20.1</v>
+      </c>
+      <c r="AA458" t="n">
+        <v>-26.2</v>
+      </c>
       <c r="AB458" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="AC458" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AD458" t="n">
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="AE458" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF458" t="inlineStr"/>
-      <c r="AG458" t="inlineStr"/>
+        <v>0.5</v>
+      </c>
+      <c r="AF458" t="n">
+        <v>162744.7</v>
+      </c>
+      <c r="AG458" t="n">
+        <v>78201.89999999999</v>
+      </c>
       <c r="AH458" t="inlineStr"/>
       <c r="AI458" t="inlineStr"/>
       <c r="AJ458" t="inlineStr"/>
@@ -57266,10 +57274,10 @@
         <v>1.2</v>
       </c>
       <c r="N459" t="n">
-        <v>-0.1</v>
+        <v>555.2</v>
       </c>
       <c r="O459" t="n">
-        <v>0</v>
+        <v>90.5</v>
       </c>
       <c r="P459" t="n">
         <v>39.77</v>
@@ -57299,47 +57307,49 @@
         <v>1.3</v>
       </c>
       <c r="Y459" t="n">
-        <v>-0.1</v>
+        <v>522.9</v>
       </c>
       <c r="Z459" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA459" t="inlineStr"/>
+        <v>78</v>
+      </c>
+      <c r="AA459" t="n">
+        <v>128.8</v>
+      </c>
       <c r="AB459" t="n">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="AC459" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="AD459" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="AE459" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AF459" t="n">
+        <v>80521.39999999999</v>
+      </c>
+      <c r="AG459" t="n">
+        <v>35058.8</v>
+      </c>
+      <c r="AH459" t="n">
+        <v>663.2</v>
+      </c>
+      <c r="AI459" t="n">
+        <v>7.7</v>
+      </c>
+      <c r="AJ459" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="AK459" t="n">
         <v>1</v>
       </c>
-      <c r="AE459" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF459" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG459" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH459" t="n">
-        <v>-0.1</v>
-      </c>
-      <c r="AI459" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ459" t="n">
-        <v>1</v>
-      </c>
-      <c r="AK459" t="n">
-        <v>0</v>
-      </c>
       <c r="AL459" t="n">
-        <v>0</v>
+        <v>2.1</v>
       </c>
       <c r="AM459" t="n">
-        <v>0</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="460">
@@ -57393,10 +57403,10 @@
         <v>1.4</v>
       </c>
       <c r="N460" t="n">
-        <v>-0</v>
+        <v>340.2</v>
       </c>
       <c r="O460" t="n">
-        <v>0</v>
+        <v>14.7</v>
       </c>
       <c r="P460" t="n">
         <v>46.6</v>
@@ -57426,47 +57436,49 @@
         <v>3.6</v>
       </c>
       <c r="Y460" t="n">
-        <v>-0</v>
+        <v>337</v>
       </c>
       <c r="Z460" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA460" t="inlineStr"/>
+        <v>11.4</v>
+      </c>
+      <c r="AA460" t="n">
+        <v>13.8</v>
+      </c>
       <c r="AB460" t="n">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AC460" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AD460" t="n">
-        <v>1</v>
+        <v>4.5</v>
       </c>
       <c r="AE460" t="n">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="AF460" t="n">
-        <v>0</v>
+        <v>29202.4</v>
       </c>
       <c r="AG460" t="n">
-        <v>0</v>
+        <v>13078.8</v>
       </c>
       <c r="AH460" t="n">
-        <v>-0</v>
+        <v>346.3</v>
       </c>
       <c r="AI460" t="n">
-        <v>0</v>
+        <v>18.1</v>
       </c>
       <c r="AJ460" t="n">
-        <v>1</v>
+        <v>6.2</v>
       </c>
       <c r="AK460" t="n">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="AL460" t="n">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="AM460" t="n">
-        <v>0</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="461">
@@ -57520,10 +57532,10 @@
         <v>2</v>
       </c>
       <c r="N461" t="n">
-        <v>-0.1</v>
+        <v>409.2</v>
       </c>
       <c r="O461" t="n">
-        <v>0.1</v>
+        <v>36.8</v>
       </c>
       <c r="P461" t="n">
         <v>35.62</v>
@@ -57553,29 +57565,31 @@
         <v>2.2</v>
       </c>
       <c r="Y461" t="n">
-        <v>-0.1</v>
+        <v>409.2</v>
       </c>
       <c r="Z461" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="AA461" t="inlineStr"/>
+        <v>36.8</v>
+      </c>
+      <c r="AA461" t="n">
+        <v>48</v>
+      </c>
       <c r="AB461" t="n">
-        <v>0</v>
+        <v>2.1</v>
       </c>
       <c r="AC461" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD461" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="AE461" t="n">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="AF461" t="n">
-        <v>0</v>
+        <v>106848.3</v>
       </c>
       <c r="AG461" t="n">
-        <v>0</v>
+        <v>53211.8</v>
       </c>
       <c r="AH461" t="inlineStr"/>
       <c r="AI461" t="inlineStr"/>
@@ -57635,10 +57649,10 @@
         <v>0.9</v>
       </c>
       <c r="N462" t="n">
-        <v>-0</v>
+        <v>349.4</v>
       </c>
       <c r="O462" t="n">
-        <v>0</v>
+        <v>36.1</v>
       </c>
       <c r="P462" t="n">
         <v>43</v>
@@ -57668,29 +57682,31 @@
         <v>1.9</v>
       </c>
       <c r="Y462" t="n">
-        <v>-0</v>
+        <v>349.4</v>
       </c>
       <c r="Z462" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA462" t="inlineStr"/>
+        <v>36.1</v>
+      </c>
+      <c r="AA462" t="n">
+        <v>34.8</v>
+      </c>
       <c r="AB462" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AC462" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="AD462" t="n">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="AE462" t="n">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="AF462" t="n">
-        <v>0</v>
+        <v>68135.8</v>
       </c>
       <c r="AG462" t="n">
-        <v>0</v>
+        <v>68974</v>
       </c>
       <c r="AH462" t="inlineStr"/>
       <c r="AI462" t="inlineStr"/>
@@ -57750,10 +57766,10 @@
         <v>2.2</v>
       </c>
       <c r="N463" t="n">
-        <v>-0.1</v>
+        <v>491.2</v>
       </c>
       <c r="O463" t="n">
-        <v>0</v>
+        <v>31.3</v>
       </c>
       <c r="P463" t="n">
         <v>29.32</v>
@@ -57783,29 +57799,31 @@
         <v>6.2</v>
       </c>
       <c r="Y463" t="n">
-        <v>-0.1</v>
+        <v>491.2</v>
       </c>
       <c r="Z463" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA463" t="inlineStr"/>
+        <v>31.3</v>
+      </c>
+      <c r="AA463" t="n">
+        <v>-33.4</v>
+      </c>
       <c r="AB463" t="n">
-        <v>0</v>
+        <v>4.1</v>
       </c>
       <c r="AC463" t="n">
-        <v>0</v>
+        <v>3.4</v>
       </c>
       <c r="AD463" t="n">
-        <v>1</v>
+        <v>10.1</v>
       </c>
       <c r="AE463" t="n">
-        <v>0</v>
+        <v>8.1</v>
       </c>
       <c r="AF463" t="n">
-        <v>0</v>
+        <v>160667.3</v>
       </c>
       <c r="AG463" t="n">
-        <v>0</v>
+        <v>174413</v>
       </c>
       <c r="AH463" t="inlineStr"/>
       <c r="AI463" t="inlineStr"/>
@@ -57865,10 +57883,10 @@
         <v>7.7</v>
       </c>
       <c r="N464" t="n">
-        <v>-0.1</v>
+        <v>527</v>
       </c>
       <c r="O464" t="n">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="P464" t="n">
         <v>36.95</v>
@@ -57898,47 +57916,49 @@
         <v>9.699999999999999</v>
       </c>
       <c r="Y464" t="n">
-        <v>-0.1</v>
+        <v>523.5</v>
       </c>
       <c r="Z464" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA464" t="inlineStr"/>
+        <v>40.6</v>
+      </c>
+      <c r="AA464" t="n">
+        <v>5.9</v>
+      </c>
       <c r="AB464" t="n">
-        <v>0</v>
+        <v>2.2</v>
       </c>
       <c r="AC464" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD464" t="n">
-        <v>1</v>
+        <v>4.5</v>
       </c>
       <c r="AE464" t="n">
-        <v>0</v>
+        <v>4.3</v>
       </c>
       <c r="AF464" t="n">
-        <v>0</v>
+        <v>92262.10000000001</v>
       </c>
       <c r="AG464" t="n">
-        <v>0</v>
+        <v>103896.8</v>
       </c>
       <c r="AH464" t="n">
-        <v>-0.1</v>
+        <v>548.5</v>
       </c>
       <c r="AI464" t="n">
-        <v>0</v>
+        <v>43.8</v>
       </c>
       <c r="AJ464" t="n">
-        <v>1</v>
+        <v>21.2</v>
       </c>
       <c r="AK464" t="n">
-        <v>0</v>
+        <v>11.2</v>
       </c>
       <c r="AL464" t="n">
-        <v>0</v>
+        <v>10.4</v>
       </c>
       <c r="AM464" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="465">
@@ -57991,8 +58011,12 @@
       <c r="M465" t="n">
         <v>1.3</v>
       </c>
-      <c r="N465" t="inlineStr"/>
-      <c r="O465" t="inlineStr"/>
+      <c r="N465" t="n">
+        <v>464.9</v>
+      </c>
+      <c r="O465" t="n">
+        <v>25.2</v>
+      </c>
       <c r="P465" t="n">
         <v>31.37</v>
       </c>
@@ -58020,15 +58044,33 @@
       <c r="X465" t="n">
         <v>2</v>
       </c>
-      <c r="Y465" t="inlineStr"/>
-      <c r="Z465" t="inlineStr"/>
-      <c r="AA465" t="inlineStr"/>
-      <c r="AB465" t="inlineStr"/>
-      <c r="AC465" t="inlineStr"/>
-      <c r="AD465" t="inlineStr"/>
-      <c r="AE465" t="inlineStr"/>
-      <c r="AF465" t="inlineStr"/>
-      <c r="AG465" t="inlineStr"/>
+      <c r="Y465" t="n">
+        <v>464.9</v>
+      </c>
+      <c r="Z465" t="n">
+        <v>25.2</v>
+      </c>
+      <c r="AA465" t="n">
+        <v>29.5</v>
+      </c>
+      <c r="AB465" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AC465" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AD465" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="AE465" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="AF465" t="n">
+        <v>103313.2</v>
+      </c>
+      <c r="AG465" t="n">
+        <v>31166.8</v>
+      </c>
       <c r="AH465" t="inlineStr"/>
       <c r="AI465" t="inlineStr"/>
       <c r="AJ465" t="inlineStr"/>
@@ -58087,10 +58129,10 @@
         <v>1.5</v>
       </c>
       <c r="N466" t="n">
-        <v>-0</v>
+        <v>328.1</v>
       </c>
       <c r="O466" t="n">
-        <v>0</v>
+        <v>16.6</v>
       </c>
       <c r="P466" t="n">
         <v>16.73</v>
@@ -58120,29 +58162,31 @@
         <v>2</v>
       </c>
       <c r="Y466" t="n">
-        <v>-0</v>
+        <v>328.1</v>
       </c>
       <c r="Z466" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA466" t="inlineStr"/>
+        <v>16.6</v>
+      </c>
+      <c r="AA466" t="n">
+        <v>15.3</v>
+      </c>
       <c r="AB466" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC466" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="AD466" t="n">
-        <v>1</v>
+        <v>5.2</v>
       </c>
       <c r="AE466" t="n">
-        <v>0</v>
+        <v>1.7</v>
       </c>
       <c r="AF466" t="n">
-        <v>0</v>
+        <v>40842.2</v>
       </c>
       <c r="AG466" t="n">
-        <v>0</v>
+        <v>19452.4</v>
       </c>
       <c r="AH466" t="inlineStr"/>
       <c r="AI466" t="inlineStr"/>
@@ -58202,10 +58246,10 @@
         <v>4.2</v>
       </c>
       <c r="N467" t="n">
-        <v>-0.1</v>
+        <v>363</v>
       </c>
       <c r="O467" t="n">
-        <v>0</v>
+        <v>55.1</v>
       </c>
       <c r="P467" t="n">
         <v>58.45</v>
@@ -58235,47 +58279,49 @@
         <v>5.9</v>
       </c>
       <c r="Y467" t="n">
-        <v>0</v>
+        <v>343.8</v>
       </c>
       <c r="Z467" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA467" t="inlineStr"/>
+        <v>48.5</v>
+      </c>
+      <c r="AA467" t="n">
+        <v>71</v>
+      </c>
       <c r="AB467" t="n">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="AC467" t="n">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="AD467" t="n">
-        <v>1</v>
+        <v>3.6</v>
       </c>
       <c r="AE467" t="n">
-        <v>0</v>
+        <v>2.1</v>
       </c>
       <c r="AF467" t="n">
-        <v>0</v>
+        <v>17794.4</v>
       </c>
       <c r="AG467" t="n">
-        <v>0</v>
+        <v>6225.6</v>
       </c>
       <c r="AH467" t="n">
-        <v>-0.1</v>
+        <v>424.3</v>
       </c>
       <c r="AI467" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="AJ467" t="n">
-        <v>1</v>
+        <v>17.8</v>
       </c>
       <c r="AK467" t="n">
-        <v>0</v>
+        <v>8.4</v>
       </c>
       <c r="AL467" t="n">
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="AM467" t="n">
-        <v>0</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="468">
@@ -58329,10 +58375,10 @@
         <v>1.8</v>
       </c>
       <c r="N468" t="n">
-        <v>-0</v>
+        <v>387</v>
       </c>
       <c r="O468" t="n">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="P468" t="n">
         <v>35.38</v>
@@ -58362,43 +58408,49 @@
         <v>3.2</v>
       </c>
       <c r="Y468" t="n">
-        <v>0.1</v>
+        <v>375.6</v>
       </c>
       <c r="Z468" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA468" t="inlineStr"/>
+        <v>38.7</v>
+      </c>
+      <c r="AA468" t="n">
+        <v>59.5</v>
+      </c>
       <c r="AB468" t="n">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AC468" t="n">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="AD468" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="AE468" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="AF468" t="n">
+        <v>25904.9</v>
+      </c>
+      <c r="AG468" t="n">
+        <v>12150.1</v>
+      </c>
+      <c r="AH468" t="n">
+        <v>407.8</v>
+      </c>
+      <c r="AI468" t="n">
+        <v>53.4</v>
+      </c>
+      <c r="AJ468" t="n">
+        <v>11.4</v>
+      </c>
+      <c r="AK468" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="AL468" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="AM468" t="n">
         <v>1</v>
-      </c>
-      <c r="AE468" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF468" t="inlineStr"/>
-      <c r="AG468" t="inlineStr"/>
-      <c r="AH468" t="n">
-        <v>-0</v>
-      </c>
-      <c r="AI468" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ468" t="n">
-        <v>1</v>
-      </c>
-      <c r="AK468" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL468" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM468" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="469">
@@ -58452,10 +58504,10 @@
         <v>2.4</v>
       </c>
       <c r="N469" t="n">
-        <v>-0.1</v>
+        <v>478.4</v>
       </c>
       <c r="O469" t="n">
-        <v>0</v>
+        <v>45.6</v>
       </c>
       <c r="P469" t="n">
         <v>17.17</v>
@@ -58485,43 +58537,49 @@
         <v>5.3</v>
       </c>
       <c r="Y469" t="n">
-        <v>-0.1</v>
+        <v>436.3</v>
       </c>
       <c r="Z469" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="AA469" t="inlineStr"/>
+        <v>27.2</v>
+      </c>
+      <c r="AA469" t="n">
+        <v>26.3</v>
+      </c>
       <c r="AB469" t="n">
-        <v>0</v>
+        <v>1.1</v>
       </c>
       <c r="AC469" t="n">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AD469" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AE469" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF469" t="inlineStr"/>
-      <c r="AG469" t="inlineStr"/>
+        <v>2.2</v>
+      </c>
+      <c r="AF469" t="n">
+        <v>53830.7</v>
+      </c>
+      <c r="AG469" t="n">
+        <v>18619.5</v>
+      </c>
       <c r="AH469" t="n">
-        <v>-0.1</v>
+        <v>513.8</v>
       </c>
       <c r="AI469" t="n">
-        <v>0</v>
+        <v>21.5</v>
       </c>
       <c r="AJ469" t="n">
-        <v>1</v>
+        <v>10.1</v>
       </c>
       <c r="AK469" t="n">
-        <v>0</v>
+        <v>4.4</v>
       </c>
       <c r="AL469" t="n">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="AM469" t="n">
-        <v>0</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="470">
@@ -58575,10 +58633,10 @@
         <v>1.4</v>
       </c>
       <c r="N470" t="n">
-        <v>-0</v>
+        <v>350.2</v>
       </c>
       <c r="O470" t="n">
-        <v>0</v>
+        <v>27.6</v>
       </c>
       <c r="P470" t="n">
         <v>28.42</v>
@@ -58607,32 +58665,50 @@
       <c r="X470" t="n">
         <v>0.8</v>
       </c>
-      <c r="Y470" t="inlineStr"/>
-      <c r="Z470" t="inlineStr"/>
-      <c r="AA470" t="inlineStr"/>
-      <c r="AB470" t="inlineStr"/>
-      <c r="AC470" t="inlineStr"/>
-      <c r="AD470" t="inlineStr"/>
-      <c r="AE470" t="inlineStr"/>
-      <c r="AF470" t="inlineStr"/>
-      <c r="AG470" t="inlineStr"/>
+      <c r="Y470" t="n">
+        <v>329.1</v>
+      </c>
+      <c r="Z470" t="n">
+        <v>14.3</v>
+      </c>
+      <c r="AA470" t="n">
+        <v>17.9</v>
+      </c>
+      <c r="AB470" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="AC470" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AD470" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="AE470" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="AF470" t="n">
+        <v>25736.9</v>
+      </c>
+      <c r="AG470" t="n">
+        <v>9873.1</v>
+      </c>
       <c r="AH470" t="n">
-        <v>-0</v>
+        <v>379</v>
       </c>
       <c r="AI470" t="n">
-        <v>0</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="AJ470" t="n">
-        <v>1</v>
+        <v>5.9</v>
       </c>
       <c r="AK470" t="n">
-        <v>0</v>
+        <v>1.7</v>
       </c>
       <c r="AL470" t="n">
-        <v>0</v>
+        <v>1.4</v>
       </c>
       <c r="AM470" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="471">
@@ -58686,10 +58762,10 @@
         <v>7.3</v>
       </c>
       <c r="N471" t="n">
-        <v>-0.1</v>
+        <v>587</v>
       </c>
       <c r="O471" t="n">
-        <v>0</v>
+        <v>66.90000000000001</v>
       </c>
       <c r="P471" t="n">
         <v>22.55</v>
@@ -58719,47 +58795,49 @@
         <v>4.7</v>
       </c>
       <c r="Y471" t="n">
-        <v>-0.1</v>
+        <v>617.7</v>
       </c>
       <c r="Z471" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA471" t="inlineStr"/>
+        <v>42.1</v>
+      </c>
+      <c r="AA471" t="n">
+        <v>-49.7</v>
+      </c>
       <c r="AB471" t="n">
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="AC471" t="n">
-        <v>0</v>
+        <v>2.8</v>
       </c>
       <c r="AD471" t="n">
-        <v>1</v>
+        <v>4.4</v>
       </c>
       <c r="AE471" t="n">
-        <v>0</v>
+        <v>4.8</v>
       </c>
       <c r="AF471" t="n">
-        <v>0.1</v>
+        <v>82562.3</v>
       </c>
       <c r="AG471" t="n">
-        <v>0.1</v>
+        <v>118371</v>
       </c>
       <c r="AH471" t="n">
-        <v>-0.1</v>
+        <v>493.9</v>
       </c>
       <c r="AI471" t="n">
-        <v>0</v>
+        <v>34.4</v>
       </c>
       <c r="AJ471" t="n">
-        <v>1</v>
+        <v>20.5</v>
       </c>
       <c r="AK471" t="n">
-        <v>0</v>
+        <v>8.1</v>
       </c>
       <c r="AL471" t="n">
-        <v>0</v>
+        <v>8.6</v>
       </c>
       <c r="AM471" t="n">
-        <v>0</v>
+        <v>4.1</v>
       </c>
     </row>
     <row r="472">
@@ -58813,10 +58891,10 @@
         <v>1.2</v>
       </c>
       <c r="N472" t="n">
-        <v>-0.1</v>
+        <v>477.3</v>
       </c>
       <c r="O472" t="n">
-        <v>0.1</v>
+        <v>84.5</v>
       </c>
       <c r="P472" t="n">
         <v>56.45</v>
@@ -58846,29 +58924,31 @@
         <v>4</v>
       </c>
       <c r="Y472" t="n">
-        <v>-0.1</v>
+        <v>477.3</v>
       </c>
       <c r="Z472" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="AA472" t="inlineStr"/>
+        <v>84.5</v>
+      </c>
+      <c r="AA472" t="n">
+        <v>117.1</v>
+      </c>
       <c r="AB472" t="n">
-        <v>0</v>
+        <v>2.3</v>
       </c>
       <c r="AC472" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD472" t="n">
-        <v>1</v>
+        <v>5.6</v>
       </c>
       <c r="AE472" t="n">
-        <v>0</v>
+        <v>3.3</v>
       </c>
       <c r="AF472" t="n">
-        <v>0</v>
+        <v>49760.8</v>
       </c>
       <c r="AG472" t="n">
-        <v>0</v>
+        <v>32669.5</v>
       </c>
       <c r="AH472" t="inlineStr"/>
       <c r="AI472" t="inlineStr"/>
@@ -58928,10 +59008,10 @@
         <v>1.7</v>
       </c>
       <c r="N473" t="n">
-        <v>-0.1</v>
+        <v>413.8</v>
       </c>
       <c r="O473" t="n">
-        <v>0</v>
+        <v>27.1</v>
       </c>
       <c r="P473" t="n">
         <v>44.25</v>
@@ -58961,47 +59041,49 @@
         <v>4.8</v>
       </c>
       <c r="Y473" t="n">
-        <v>-0.1</v>
+        <v>419.1</v>
       </c>
       <c r="Z473" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA473" t="inlineStr"/>
+        <v>25.9</v>
+      </c>
+      <c r="AA473" t="n">
+        <v>5</v>
+      </c>
       <c r="AB473" t="n">
-        <v>0</v>
+        <v>3.8</v>
       </c>
       <c r="AC473" t="n">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="AD473" t="n">
-        <v>1</v>
+        <v>11.4</v>
       </c>
       <c r="AE473" t="n">
-        <v>0</v>
+        <v>2.2</v>
       </c>
       <c r="AF473" t="n">
-        <v>0</v>
+        <v>107890.5</v>
       </c>
       <c r="AG473" t="n">
-        <v>0</v>
+        <v>49789.9</v>
       </c>
       <c r="AH473" t="n">
-        <v>-0.1</v>
+        <v>391.3</v>
       </c>
       <c r="AI473" t="n">
-        <v>0</v>
+        <v>19.7</v>
       </c>
       <c r="AJ473" t="n">
-        <v>1</v>
+        <v>12.1</v>
       </c>
       <c r="AK473" t="n">
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="AL473" t="n">
-        <v>0</v>
+        <v>3.2</v>
       </c>
       <c r="AM473" t="n">
-        <v>0</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="474">
@@ -59054,8 +59136,12 @@
       <c r="M474" t="n">
         <v>5.7</v>
       </c>
-      <c r="N474" t="inlineStr"/>
-      <c r="O474" t="inlineStr"/>
+      <c r="N474" t="n">
+        <v>506.8</v>
+      </c>
+      <c r="O474" t="n">
+        <v>55</v>
+      </c>
       <c r="P474" t="n">
         <v>59.28</v>
       </c>
@@ -59083,17 +59169,31 @@
       <c r="X474" t="n">
         <v>4.4</v>
       </c>
-      <c r="Y474" t="inlineStr"/>
-      <c r="Z474" t="inlineStr"/>
-      <c r="AA474" t="inlineStr"/>
+      <c r="Y474" t="n">
+        <v>493.1</v>
+      </c>
+      <c r="Z474" t="n">
+        <v>37</v>
+      </c>
+      <c r="AA474" t="n">
+        <v>73.40000000000001</v>
+      </c>
       <c r="AB474" t="inlineStr"/>
       <c r="AC474" t="inlineStr"/>
       <c r="AD474" t="inlineStr"/>
       <c r="AE474" t="inlineStr"/>
-      <c r="AF474" t="inlineStr"/>
-      <c r="AG474" t="inlineStr"/>
-      <c r="AH474" t="inlineStr"/>
-      <c r="AI474" t="inlineStr"/>
+      <c r="AF474" t="n">
+        <v>95986.2</v>
+      </c>
+      <c r="AG474" t="n">
+        <v>63935.3</v>
+      </c>
+      <c r="AH474" t="n">
+        <v>598</v>
+      </c>
+      <c r="AI474" t="n">
+        <v>66.59999999999999</v>
+      </c>
       <c r="AJ474" t="inlineStr"/>
       <c r="AK474" t="inlineStr"/>
       <c r="AL474" t="inlineStr"/>
@@ -59150,7 +59250,7 @@
         <v>19.8</v>
       </c>
       <c r="N475" t="n">
-        <v>-0.2</v>
+        <v>398</v>
       </c>
       <c r="O475" t="n">
         <v>0</v>
@@ -59183,44 +59283,46 @@
         <v>19.2</v>
       </c>
       <c r="Y475" t="n">
-        <v>-0.2</v>
+        <v>398</v>
       </c>
       <c r="Z475" t="n">
         <v>0</v>
       </c>
-      <c r="AA475" t="inlineStr"/>
+      <c r="AA475" t="n">
+        <v>0</v>
+      </c>
       <c r="AB475" t="n">
-        <v>0</v>
+        <v>1.4</v>
       </c>
       <c r="AC475" t="n">
         <v>0</v>
       </c>
       <c r="AD475" t="n">
-        <v>1</v>
+        <v>5.3</v>
       </c>
       <c r="AE475" t="n">
         <v>0</v>
       </c>
       <c r="AF475" t="n">
-        <v>0</v>
+        <v>143000</v>
       </c>
       <c r="AG475" t="n">
         <v>0</v>
       </c>
       <c r="AH475" t="n">
-        <v>-0.2</v>
+        <v>398</v>
       </c>
       <c r="AI475" t="n">
         <v>0</v>
       </c>
       <c r="AJ475" t="n">
-        <v>1</v>
+        <v>5.3</v>
       </c>
       <c r="AK475" t="n">
         <v>0</v>
       </c>
       <c r="AL475" t="n">
-        <v>0</v>
+        <v>1.4</v>
       </c>
       <c r="AM475" t="n">
         <v>0</v>
@@ -76377,10 +76479,10 @@
         <v>1.9</v>
       </c>
       <c r="N656" t="n">
-        <v>0</v>
+        <v>378.4</v>
       </c>
       <c r="O656" t="n">
-        <v>0</v>
+        <v>8.1</v>
       </c>
       <c r="P656" t="n">
         <v>23</v>
@@ -76410,19 +76512,19 @@
         <v>5</v>
       </c>
       <c r="Y656" t="n">
-        <v>0</v>
+        <v>378.4</v>
       </c>
       <c r="Z656" t="n">
-        <v>0</v>
+        <v>8.1</v>
       </c>
       <c r="AA656" t="n">
-        <v>0</v>
+        <v>12.6</v>
       </c>
       <c r="AB656" t="n">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="AC656" t="n">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="AD656" t="n">
         <v>7.6</v>
@@ -76494,10 +76596,10 @@
         <v>1.3</v>
       </c>
       <c r="N657" t="n">
-        <v>0</v>
+        <v>530.9</v>
       </c>
       <c r="O657" t="n">
-        <v>0</v>
+        <v>49.2</v>
       </c>
       <c r="P657" t="n">
         <v>38</v>
@@ -76527,19 +76629,19 @@
         <v>2</v>
       </c>
       <c r="Y657" t="n">
-        <v>0</v>
+        <v>530.9</v>
       </c>
       <c r="Z657" t="n">
-        <v>0</v>
+        <v>49.2</v>
       </c>
       <c r="AA657" t="n">
-        <v>0</v>
+        <v>-94.5</v>
       </c>
       <c r="AB657" t="n">
-        <v>0</v>
+        <v>1.6</v>
       </c>
       <c r="AC657" t="n">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="AD657" t="n">
         <v>3.6</v>
@@ -76611,10 +76713,10 @@
         <v>1.3</v>
       </c>
       <c r="N658" t="n">
-        <v>0</v>
+        <v>448.1</v>
       </c>
       <c r="O658" t="n">
-        <v>0</v>
+        <v>23.3</v>
       </c>
       <c r="P658" t="n">
         <v>28</v>
@@ -76644,19 +76746,19 @@
         <v>1.4</v>
       </c>
       <c r="Y658" t="n">
-        <v>0</v>
+        <v>459.4</v>
       </c>
       <c r="Z658" t="n">
-        <v>0</v>
+        <v>11.8</v>
       </c>
       <c r="AA658" t="n">
-        <v>0</v>
+        <v>-21.8</v>
       </c>
       <c r="AB658" t="n">
-        <v>0</v>
+        <v>1.1</v>
       </c>
       <c r="AC658" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AD658" t="n">
         <v>3.1</v>
@@ -76671,10 +76773,10 @@
         <v>43304</v>
       </c>
       <c r="AH658" t="n">
-        <v>0</v>
+        <v>413</v>
       </c>
       <c r="AI658" t="n">
-        <v>0</v>
+        <v>12.7</v>
       </c>
       <c r="AJ658" t="n">
         <v>4.6</v>
@@ -76683,10 +76785,10 @@
         <v>1.6</v>
       </c>
       <c r="AL658" t="n">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="AM658" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="659">
@@ -76740,10 +76842,10 @@
         <v>1.6</v>
       </c>
       <c r="N659" t="n">
-        <v>0</v>
+        <v>373.5</v>
       </c>
       <c r="O659" t="n">
-        <v>0</v>
+        <v>9.1</v>
       </c>
       <c r="P659" t="n">
         <v>27</v>
@@ -76773,19 +76875,19 @@
         <v>2</v>
       </c>
       <c r="Y659" t="n">
-        <v>0</v>
+        <v>373.5</v>
       </c>
       <c r="Z659" t="n">
-        <v>0</v>
+        <v>9.1</v>
       </c>
       <c r="AA659" t="n">
-        <v>0</v>
+        <v>-13.4</v>
       </c>
       <c r="AB659" t="n">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="AC659" t="n">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="AD659" t="n">
         <v>5.6</v>
@@ -76857,10 +76959,10 @@
         <v>1</v>
       </c>
       <c r="N660" t="n">
-        <v>0</v>
+        <v>359.2</v>
       </c>
       <c r="O660" t="n">
-        <v>0</v>
+        <v>10.6</v>
       </c>
       <c r="P660" t="n">
         <v>30</v>
@@ -76890,19 +76992,19 @@
         <v>2.2</v>
       </c>
       <c r="Y660" t="n">
-        <v>0</v>
+        <v>357.5</v>
       </c>
       <c r="Z660" t="n">
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="AA660" t="n">
-        <v>0</v>
+        <v>12.2</v>
       </c>
       <c r="AB660" t="n">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AC660" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="AD660" t="n">
         <v>4.2</v>
@@ -76917,10 +77019,10 @@
         <v>27689.8</v>
       </c>
       <c r="AH660" t="n">
-        <v>0</v>
+        <v>366.3</v>
       </c>
       <c r="AI660" t="n">
-        <v>0</v>
+        <v>17.2</v>
       </c>
       <c r="AJ660" t="n">
         <v>5.6</v>
@@ -76929,10 +77031,10 @@
         <v>1.5</v>
       </c>
       <c r="AL660" t="n">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="AM660" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="661">

</xml_diff>

<commit_message>
MAVEN Huang SIRs added
</commit_message>
<xml_diff>
--- a/icmecat/HELCATS_ICMECAT_v20.xlsx
+++ b/icmecat/HELCATS_ICMECAT_v20.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="ICMECATv2.0" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ICMECATv2.0" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -54,18 +54,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -87484,6 +87484,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ICMECat update Dec 2
</commit_message>
<xml_diff>
--- a/icmecat/HELCATS_ICMECAT_v20.xlsx
+++ b/icmecat/HELCATS_ICMECAT_v20.xlsx
@@ -564,8 +564,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">ICME_STEREO_A_MOESTL_20201027_01
-</t>
+          <t>ICME_STEREO_A_MOESTL_20201027_01</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -789,8 +788,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve">ICME_STEREO_A_MOESTL_20200910_01
-</t>
+          <t>ICME_STEREO_A_MOESTL_20200910_01</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -885,8 +883,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve">ICME_STEREO_A_MOESTL_20200908_01
-</t>
+          <t>ICME_STEREO_A_MOESTL_20200908_01</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -981,8 +978,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve">ICME_STEREO_A_MOESTL_20200901_01
-</t>
+          <t>ICME_STEREO_A_MOESTL_20200901_01</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1172,8 +1168,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve">ICME_STEREO_A_MOESTL_20200819_01
-</t>
+          <t>ICME_STEREO_A_MOESTL_20200819_01</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -1268,8 +1263,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t xml:space="preserve">ICME_STEREO_A_MOESTL_20200805_01
-</t>
+          <t>ICME_STEREO_A_MOESTL_20200805_01</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">

</xml_diff>

<commit_message>
update ICMECAT 2020 Dec 3
</commit_message>
<xml_diff>
--- a/icmecat/HELCATS_ICMECAT_v20.xlsx
+++ b/icmecat/HELCATS_ICMECAT_v20.xlsx
@@ -579,7 +579,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2020-10-28T08:53Z</t>
+          <t>2020-10-28T07:58Z</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -611,7 +611,7 @@
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr"/>
       <c r="P2" t="n">
-        <v>21.98</v>
+        <v>22.9</v>
       </c>
       <c r="Q2" t="n">
         <v>8.699999999999999</v>
@@ -632,10 +632,10 @@
         <v>0.8</v>
       </c>
       <c r="W2" t="n">
-        <v>2.5</v>
+        <v>2.3</v>
       </c>
       <c r="X2" t="n">
-        <v>2.5</v>
+        <v>2.6</v>
       </c>
       <c r="Y2" t="inlineStr"/>
       <c r="Z2" t="inlineStr"/>
@@ -798,7 +798,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2020-09-10T04:11Z</t>
+          <t>2020-09-10T02:50Z</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -821,16 +821,16 @@
         <v>3.64</v>
       </c>
       <c r="J4" t="n">
-        <v>6.72</v>
+        <v>8.07</v>
       </c>
       <c r="K4" t="n">
         <v>10.9</v>
       </c>
       <c r="L4" t="n">
-        <v>9.199999999999999</v>
+        <v>9.1</v>
       </c>
       <c r="M4" t="n">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr"/>
@@ -893,12 +893,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2020-09-08T14:47Z</t>
+          <t>2020-09-08T05:28Z</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2020-09-08T14:47Z</t>
+          <t>2020-09-08T12:36Z</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -913,48 +913,48 @@
         <v>-63.11</v>
       </c>
       <c r="I5" t="n">
-        <v>3.45</v>
+        <v>3.44</v>
       </c>
       <c r="J5" t="n">
-        <v>10.52</v>
+        <v>19.83</v>
       </c>
       <c r="K5" t="n">
         <v>10.8</v>
       </c>
       <c r="L5" t="n">
-        <v>9.1</v>
+        <v>7.9</v>
       </c>
       <c r="M5" t="n">
-        <v>0.6</v>
+        <v>2</v>
       </c>
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="inlineStr"/>
       <c r="P5" t="n">
-        <v>10.52</v>
+        <v>12.7</v>
       </c>
       <c r="Q5" t="n">
         <v>10.8</v>
       </c>
       <c r="R5" t="n">
-        <v>9.1</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="S5" t="n">
         <v>0.6</v>
       </c>
       <c r="T5" t="n">
-        <v>4.5</v>
+        <v>3.2</v>
       </c>
       <c r="U5" t="n">
-        <v>0.1</v>
+        <v>-5.4</v>
       </c>
       <c r="V5" t="n">
-        <v>2.5</v>
+        <v>3.7</v>
       </c>
       <c r="W5" t="n">
-        <v>-6.9</v>
+        <v>-7</v>
       </c>
       <c r="X5" t="n">
-        <v>1.8</v>
+        <v>1.7</v>
       </c>
       <c r="Y5" t="inlineStr"/>
       <c r="Z5" t="inlineStr"/>
@@ -1088,7 +1088,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2020-08-22T09:29Z</t>
+          <t>2020-08-22T07:37Z</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -1097,13 +1097,13 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>0.8702</v>
+        <v>0.8698</v>
       </c>
       <c r="H7" t="n">
-        <v>130.36</v>
+        <v>130.35</v>
       </c>
       <c r="I7" t="n">
-        <v>-4.1</v>
+        <v>-4.09</v>
       </c>
       <c r="J7" t="n">
         <v>31.32</v>
@@ -1120,31 +1120,31 @@
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
       <c r="P7" t="n">
-        <v>17.12</v>
+        <v>18.98</v>
       </c>
       <c r="Q7" t="n">
-        <v>15.2</v>
+        <v>15.8</v>
       </c>
       <c r="R7" t="n">
-        <v>11.4</v>
+        <v>11.7</v>
       </c>
       <c r="S7" t="n">
         <v>2.2</v>
       </c>
       <c r="T7" t="n">
-        <v>1.9</v>
+        <v>2.9</v>
       </c>
       <c r="U7" t="n">
         <v>-9.800000000000001</v>
       </c>
       <c r="V7" t="n">
-        <v>4.1</v>
+        <v>5</v>
       </c>
       <c r="W7" t="n">
-        <v>-9.699999999999999</v>
+        <v>-9.199999999999999</v>
       </c>
       <c r="X7" t="n">
-        <v>2.5</v>
+        <v>2.8</v>
       </c>
       <c r="Y7" t="inlineStr"/>
       <c r="Z7" t="inlineStr"/>
@@ -1468,7 +1468,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2020-07-25T23:11Z</t>
+          <t>2020-07-26T05:59Z</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1477,13 +1477,13 @@
         </is>
       </c>
       <c r="G11" t="n">
-        <v>0.712</v>
+        <v>0.7139</v>
       </c>
       <c r="H11" t="n">
-        <v>121.44</v>
+        <v>121.62</v>
       </c>
       <c r="I11" t="n">
-        <v>-0.36</v>
+        <v>-0.41</v>
       </c>
       <c r="J11" t="n">
         <v>24.33</v>
@@ -1500,31 +1500,31 @@
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="inlineStr"/>
       <c r="P11" t="n">
-        <v>24.33</v>
+        <v>17.53</v>
       </c>
       <c r="Q11" t="n">
-        <v>8.5</v>
+        <v>7.5</v>
       </c>
       <c r="R11" t="n">
         <v>5.9</v>
       </c>
       <c r="S11" t="n">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="T11" t="n">
-        <v>0.6</v>
+        <v>0.9</v>
       </c>
       <c r="U11" t="n">
-        <v>-6.5</v>
+        <v>-2.1</v>
       </c>
       <c r="V11" t="n">
-        <v>1.7</v>
+        <v>0.9</v>
       </c>
       <c r="W11" t="n">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="X11" t="n">
-        <v>2.4</v>
+        <v>1.2</v>
       </c>
       <c r="Y11" t="inlineStr"/>
       <c r="Z11" t="inlineStr"/>
@@ -1687,7 +1687,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2020-07-09T21:25Z</t>
+          <t>2020-07-09T14:17Z</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1710,7 +1710,7 @@
         <v>-4.25</v>
       </c>
       <c r="J13" t="n">
-        <v>29.48</v>
+        <v>36.62</v>
       </c>
       <c r="K13" t="n">
         <v>15.3</v>
@@ -1725,7 +1725,7 @@
         <v>373.6</v>
       </c>
       <c r="O13" t="n">
-        <v>32.4</v>
+        <v>29.3</v>
       </c>
       <c r="P13" t="n">
         <v>21.72</v>
@@ -1782,22 +1782,22 @@
         <v>23522.6</v>
       </c>
       <c r="AH13" t="n">
-        <v>392.8</v>
+        <v>383.5</v>
       </c>
       <c r="AI13" t="n">
-        <v>14.4</v>
+        <v>15.3</v>
       </c>
       <c r="AJ13" t="n">
-        <v>11.3</v>
+        <v>11.9</v>
       </c>
       <c r="AK13" t="n">
-        <v>3.5</v>
+        <v>2.9</v>
       </c>
       <c r="AL13" t="n">
         <v>3</v>
       </c>
       <c r="AM13" t="n">
-        <v>1.1</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="14">
@@ -2581,12 +2581,12 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2020-05-28T09:38Z</t>
+          <t>2020-05-28T08:50Z</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2020-05-28T09:38Z</t>
+          <t>2020-05-28T08:50Z</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2595,22 +2595,22 @@
         </is>
       </c>
       <c r="G21" t="n">
-        <v>0.3539</v>
+        <v>0.3546</v>
       </c>
       <c r="H21" t="n">
-        <v>147.67</v>
+        <v>147.58</v>
       </c>
       <c r="I21" t="n">
-        <v>2.48</v>
+        <v>2.49</v>
       </c>
       <c r="J21" t="n">
-        <v>5.35</v>
+        <v>6.15</v>
       </c>
       <c r="K21" t="n">
         <v>46.6</v>
       </c>
       <c r="L21" t="n">
-        <v>35.2</v>
+        <v>34.5</v>
       </c>
       <c r="M21" t="n">
         <v>5.4</v>
@@ -2618,31 +2618,31 @@
       <c r="N21" t="inlineStr"/>
       <c r="O21" t="inlineStr"/>
       <c r="P21" t="n">
-        <v>5.35</v>
+        <v>6.15</v>
       </c>
       <c r="Q21" t="n">
         <v>46.6</v>
       </c>
       <c r="R21" t="n">
-        <v>35.2</v>
+        <v>34.5</v>
       </c>
       <c r="S21" t="n">
         <v>5.4</v>
       </c>
       <c r="T21" t="n">
-        <v>22.4</v>
+        <v>18.9</v>
       </c>
       <c r="U21" t="n">
-        <v>-2.1</v>
+        <v>-19.4</v>
       </c>
       <c r="V21" t="n">
-        <v>10.8</v>
+        <v>13.9</v>
       </c>
       <c r="W21" t="n">
-        <v>-6.2</v>
+        <v>-9</v>
       </c>
       <c r="X21" t="n">
-        <v>23.7</v>
+        <v>23.2</v>
       </c>
       <c r="Y21" t="inlineStr"/>
       <c r="Z21" t="inlineStr"/>

</xml_diff>